<commit_message>
insert csdl tu excel
</commit_message>
<xml_diff>
--- a/upload/best_data.xlsx
+++ b/upload/best_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\phpexcel-demo-1.8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\best_xuly\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KHGD TIN UD" sheetId="4" r:id="rId1"/>
@@ -503,10 +503,10 @@
     </r>
   </si>
   <si>
-    <t>Nghành đào tạo: Tin học ứng dụng    Mã Nghành: 6480205</t>
-  </si>
-  <si>
     <t>Khóa học 42 (2017-2020)</t>
+  </si>
+  <si>
+    <t>Nghành đào tạo: Tin học ứng dụng    Mã Nghành: 1</t>
   </si>
 </sst>
 </file>
@@ -790,38 +790,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -845,9 +821,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -869,16 +842,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -895,6 +859,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1307,29 +1307,29 @@
   <sheetData>
     <row r="1" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
     </row>
     <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="22"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="20"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="49"/>
       <c r="F3" s="3" t="s">
         <v>90</v>
       </c>
@@ -2577,10 +2577,10 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="21"/>
+      <c r="C48" s="50"/>
       <c r="D48" s="3">
         <f>SUM(D4+D11)</f>
         <v>83</v>
@@ -2639,29 +2639,29 @@
   <sheetData>
     <row r="1" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="22"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="20"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="49"/>
       <c r="F3" s="3" t="s">
         <v>90</v>
       </c>
@@ -3828,10 +3828,10 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="21"/>
+      <c r="C48" s="50"/>
       <c r="D48" s="3">
         <f>SUM(D4+D11)</f>
         <v>83</v>
@@ -3876,2230 +3876,2235 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="25"/>
-    <col min="6" max="6" width="5.7109375" style="25" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="25" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" style="25" customWidth="1"/>
-    <col min="9" max="9" width="8" style="25" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" style="25" customWidth="1"/>
-    <col min="11" max="256" width="9.140625" style="25"/>
-    <col min="257" max="257" width="6.42578125" style="25" customWidth="1"/>
-    <col min="258" max="258" width="11.5703125" style="25" customWidth="1"/>
-    <col min="259" max="259" width="39.140625" style="25" customWidth="1"/>
-    <col min="260" max="265" width="9.140625" style="25"/>
-    <col min="266" max="266" width="10.42578125" style="25" customWidth="1"/>
-    <col min="267" max="512" width="9.140625" style="25"/>
-    <col min="513" max="513" width="6.42578125" style="25" customWidth="1"/>
-    <col min="514" max="514" width="11.5703125" style="25" customWidth="1"/>
-    <col min="515" max="515" width="39.140625" style="25" customWidth="1"/>
-    <col min="516" max="521" width="9.140625" style="25"/>
-    <col min="522" max="522" width="10.42578125" style="25" customWidth="1"/>
-    <col min="523" max="768" width="9.140625" style="25"/>
-    <col min="769" max="769" width="6.42578125" style="25" customWidth="1"/>
-    <col min="770" max="770" width="11.5703125" style="25" customWidth="1"/>
-    <col min="771" max="771" width="39.140625" style="25" customWidth="1"/>
-    <col min="772" max="777" width="9.140625" style="25"/>
-    <col min="778" max="778" width="10.42578125" style="25" customWidth="1"/>
-    <col min="779" max="1024" width="9.140625" style="25"/>
-    <col min="1025" max="1025" width="6.42578125" style="25" customWidth="1"/>
-    <col min="1026" max="1026" width="11.5703125" style="25" customWidth="1"/>
-    <col min="1027" max="1027" width="39.140625" style="25" customWidth="1"/>
-    <col min="1028" max="1033" width="9.140625" style="25"/>
-    <col min="1034" max="1034" width="10.42578125" style="25" customWidth="1"/>
-    <col min="1035" max="1280" width="9.140625" style="25"/>
-    <col min="1281" max="1281" width="6.42578125" style="25" customWidth="1"/>
-    <col min="1282" max="1282" width="11.5703125" style="25" customWidth="1"/>
-    <col min="1283" max="1283" width="39.140625" style="25" customWidth="1"/>
-    <col min="1284" max="1289" width="9.140625" style="25"/>
-    <col min="1290" max="1290" width="10.42578125" style="25" customWidth="1"/>
-    <col min="1291" max="1536" width="9.140625" style="25"/>
-    <col min="1537" max="1537" width="6.42578125" style="25" customWidth="1"/>
-    <col min="1538" max="1538" width="11.5703125" style="25" customWidth="1"/>
-    <col min="1539" max="1539" width="39.140625" style="25" customWidth="1"/>
-    <col min="1540" max="1545" width="9.140625" style="25"/>
-    <col min="1546" max="1546" width="10.42578125" style="25" customWidth="1"/>
-    <col min="1547" max="1792" width="9.140625" style="25"/>
-    <col min="1793" max="1793" width="6.42578125" style="25" customWidth="1"/>
-    <col min="1794" max="1794" width="11.5703125" style="25" customWidth="1"/>
-    <col min="1795" max="1795" width="39.140625" style="25" customWidth="1"/>
-    <col min="1796" max="1801" width="9.140625" style="25"/>
-    <col min="1802" max="1802" width="10.42578125" style="25" customWidth="1"/>
-    <col min="1803" max="2048" width="9.140625" style="25"/>
-    <col min="2049" max="2049" width="6.42578125" style="25" customWidth="1"/>
-    <col min="2050" max="2050" width="11.5703125" style="25" customWidth="1"/>
-    <col min="2051" max="2051" width="39.140625" style="25" customWidth="1"/>
-    <col min="2052" max="2057" width="9.140625" style="25"/>
-    <col min="2058" max="2058" width="10.42578125" style="25" customWidth="1"/>
-    <col min="2059" max="2304" width="9.140625" style="25"/>
-    <col min="2305" max="2305" width="6.42578125" style="25" customWidth="1"/>
-    <col min="2306" max="2306" width="11.5703125" style="25" customWidth="1"/>
-    <col min="2307" max="2307" width="39.140625" style="25" customWidth="1"/>
-    <col min="2308" max="2313" width="9.140625" style="25"/>
-    <col min="2314" max="2314" width="10.42578125" style="25" customWidth="1"/>
-    <col min="2315" max="2560" width="9.140625" style="25"/>
-    <col min="2561" max="2561" width="6.42578125" style="25" customWidth="1"/>
-    <col min="2562" max="2562" width="11.5703125" style="25" customWidth="1"/>
-    <col min="2563" max="2563" width="39.140625" style="25" customWidth="1"/>
-    <col min="2564" max="2569" width="9.140625" style="25"/>
-    <col min="2570" max="2570" width="10.42578125" style="25" customWidth="1"/>
-    <col min="2571" max="2816" width="9.140625" style="25"/>
-    <col min="2817" max="2817" width="6.42578125" style="25" customWidth="1"/>
-    <col min="2818" max="2818" width="11.5703125" style="25" customWidth="1"/>
-    <col min="2819" max="2819" width="39.140625" style="25" customWidth="1"/>
-    <col min="2820" max="2825" width="9.140625" style="25"/>
-    <col min="2826" max="2826" width="10.42578125" style="25" customWidth="1"/>
-    <col min="2827" max="3072" width="9.140625" style="25"/>
-    <col min="3073" max="3073" width="6.42578125" style="25" customWidth="1"/>
-    <col min="3074" max="3074" width="11.5703125" style="25" customWidth="1"/>
-    <col min="3075" max="3075" width="39.140625" style="25" customWidth="1"/>
-    <col min="3076" max="3081" width="9.140625" style="25"/>
-    <col min="3082" max="3082" width="10.42578125" style="25" customWidth="1"/>
-    <col min="3083" max="3328" width="9.140625" style="25"/>
-    <col min="3329" max="3329" width="6.42578125" style="25" customWidth="1"/>
-    <col min="3330" max="3330" width="11.5703125" style="25" customWidth="1"/>
-    <col min="3331" max="3331" width="39.140625" style="25" customWidth="1"/>
-    <col min="3332" max="3337" width="9.140625" style="25"/>
-    <col min="3338" max="3338" width="10.42578125" style="25" customWidth="1"/>
-    <col min="3339" max="3584" width="9.140625" style="25"/>
-    <col min="3585" max="3585" width="6.42578125" style="25" customWidth="1"/>
-    <col min="3586" max="3586" width="11.5703125" style="25" customWidth="1"/>
-    <col min="3587" max="3587" width="39.140625" style="25" customWidth="1"/>
-    <col min="3588" max="3593" width="9.140625" style="25"/>
-    <col min="3594" max="3594" width="10.42578125" style="25" customWidth="1"/>
-    <col min="3595" max="3840" width="9.140625" style="25"/>
-    <col min="3841" max="3841" width="6.42578125" style="25" customWidth="1"/>
-    <col min="3842" max="3842" width="11.5703125" style="25" customWidth="1"/>
-    <col min="3843" max="3843" width="39.140625" style="25" customWidth="1"/>
-    <col min="3844" max="3849" width="9.140625" style="25"/>
-    <col min="3850" max="3850" width="10.42578125" style="25" customWidth="1"/>
-    <col min="3851" max="4096" width="9.140625" style="25"/>
-    <col min="4097" max="4097" width="6.42578125" style="25" customWidth="1"/>
-    <col min="4098" max="4098" width="11.5703125" style="25" customWidth="1"/>
-    <col min="4099" max="4099" width="39.140625" style="25" customWidth="1"/>
-    <col min="4100" max="4105" width="9.140625" style="25"/>
-    <col min="4106" max="4106" width="10.42578125" style="25" customWidth="1"/>
-    <col min="4107" max="4352" width="9.140625" style="25"/>
-    <col min="4353" max="4353" width="6.42578125" style="25" customWidth="1"/>
-    <col min="4354" max="4354" width="11.5703125" style="25" customWidth="1"/>
-    <col min="4355" max="4355" width="39.140625" style="25" customWidth="1"/>
-    <col min="4356" max="4361" width="9.140625" style="25"/>
-    <col min="4362" max="4362" width="10.42578125" style="25" customWidth="1"/>
-    <col min="4363" max="4608" width="9.140625" style="25"/>
-    <col min="4609" max="4609" width="6.42578125" style="25" customWidth="1"/>
-    <col min="4610" max="4610" width="11.5703125" style="25" customWidth="1"/>
-    <col min="4611" max="4611" width="39.140625" style="25" customWidth="1"/>
-    <col min="4612" max="4617" width="9.140625" style="25"/>
-    <col min="4618" max="4618" width="10.42578125" style="25" customWidth="1"/>
-    <col min="4619" max="4864" width="9.140625" style="25"/>
-    <col min="4865" max="4865" width="6.42578125" style="25" customWidth="1"/>
-    <col min="4866" max="4866" width="11.5703125" style="25" customWidth="1"/>
-    <col min="4867" max="4867" width="39.140625" style="25" customWidth="1"/>
-    <col min="4868" max="4873" width="9.140625" style="25"/>
-    <col min="4874" max="4874" width="10.42578125" style="25" customWidth="1"/>
-    <col min="4875" max="5120" width="9.140625" style="25"/>
-    <col min="5121" max="5121" width="6.42578125" style="25" customWidth="1"/>
-    <col min="5122" max="5122" width="11.5703125" style="25" customWidth="1"/>
-    <col min="5123" max="5123" width="39.140625" style="25" customWidth="1"/>
-    <col min="5124" max="5129" width="9.140625" style="25"/>
-    <col min="5130" max="5130" width="10.42578125" style="25" customWidth="1"/>
-    <col min="5131" max="5376" width="9.140625" style="25"/>
-    <col min="5377" max="5377" width="6.42578125" style="25" customWidth="1"/>
-    <col min="5378" max="5378" width="11.5703125" style="25" customWidth="1"/>
-    <col min="5379" max="5379" width="39.140625" style="25" customWidth="1"/>
-    <col min="5380" max="5385" width="9.140625" style="25"/>
-    <col min="5386" max="5386" width="10.42578125" style="25" customWidth="1"/>
-    <col min="5387" max="5632" width="9.140625" style="25"/>
-    <col min="5633" max="5633" width="6.42578125" style="25" customWidth="1"/>
-    <col min="5634" max="5634" width="11.5703125" style="25" customWidth="1"/>
-    <col min="5635" max="5635" width="39.140625" style="25" customWidth="1"/>
-    <col min="5636" max="5641" width="9.140625" style="25"/>
-    <col min="5642" max="5642" width="10.42578125" style="25" customWidth="1"/>
-    <col min="5643" max="5888" width="9.140625" style="25"/>
-    <col min="5889" max="5889" width="6.42578125" style="25" customWidth="1"/>
-    <col min="5890" max="5890" width="11.5703125" style="25" customWidth="1"/>
-    <col min="5891" max="5891" width="39.140625" style="25" customWidth="1"/>
-    <col min="5892" max="5897" width="9.140625" style="25"/>
-    <col min="5898" max="5898" width="10.42578125" style="25" customWidth="1"/>
-    <col min="5899" max="6144" width="9.140625" style="25"/>
-    <col min="6145" max="6145" width="6.42578125" style="25" customWidth="1"/>
-    <col min="6146" max="6146" width="11.5703125" style="25" customWidth="1"/>
-    <col min="6147" max="6147" width="39.140625" style="25" customWidth="1"/>
-    <col min="6148" max="6153" width="9.140625" style="25"/>
-    <col min="6154" max="6154" width="10.42578125" style="25" customWidth="1"/>
-    <col min="6155" max="6400" width="9.140625" style="25"/>
-    <col min="6401" max="6401" width="6.42578125" style="25" customWidth="1"/>
-    <col min="6402" max="6402" width="11.5703125" style="25" customWidth="1"/>
-    <col min="6403" max="6403" width="39.140625" style="25" customWidth="1"/>
-    <col min="6404" max="6409" width="9.140625" style="25"/>
-    <col min="6410" max="6410" width="10.42578125" style="25" customWidth="1"/>
-    <col min="6411" max="6656" width="9.140625" style="25"/>
-    <col min="6657" max="6657" width="6.42578125" style="25" customWidth="1"/>
-    <col min="6658" max="6658" width="11.5703125" style="25" customWidth="1"/>
-    <col min="6659" max="6659" width="39.140625" style="25" customWidth="1"/>
-    <col min="6660" max="6665" width="9.140625" style="25"/>
-    <col min="6666" max="6666" width="10.42578125" style="25" customWidth="1"/>
-    <col min="6667" max="6912" width="9.140625" style="25"/>
-    <col min="6913" max="6913" width="6.42578125" style="25" customWidth="1"/>
-    <col min="6914" max="6914" width="11.5703125" style="25" customWidth="1"/>
-    <col min="6915" max="6915" width="39.140625" style="25" customWidth="1"/>
-    <col min="6916" max="6921" width="9.140625" style="25"/>
-    <col min="6922" max="6922" width="10.42578125" style="25" customWidth="1"/>
-    <col min="6923" max="7168" width="9.140625" style="25"/>
-    <col min="7169" max="7169" width="6.42578125" style="25" customWidth="1"/>
-    <col min="7170" max="7170" width="11.5703125" style="25" customWidth="1"/>
-    <col min="7171" max="7171" width="39.140625" style="25" customWidth="1"/>
-    <col min="7172" max="7177" width="9.140625" style="25"/>
-    <col min="7178" max="7178" width="10.42578125" style="25" customWidth="1"/>
-    <col min="7179" max="7424" width="9.140625" style="25"/>
-    <col min="7425" max="7425" width="6.42578125" style="25" customWidth="1"/>
-    <col min="7426" max="7426" width="11.5703125" style="25" customWidth="1"/>
-    <col min="7427" max="7427" width="39.140625" style="25" customWidth="1"/>
-    <col min="7428" max="7433" width="9.140625" style="25"/>
-    <col min="7434" max="7434" width="10.42578125" style="25" customWidth="1"/>
-    <col min="7435" max="7680" width="9.140625" style="25"/>
-    <col min="7681" max="7681" width="6.42578125" style="25" customWidth="1"/>
-    <col min="7682" max="7682" width="11.5703125" style="25" customWidth="1"/>
-    <col min="7683" max="7683" width="39.140625" style="25" customWidth="1"/>
-    <col min="7684" max="7689" width="9.140625" style="25"/>
-    <col min="7690" max="7690" width="10.42578125" style="25" customWidth="1"/>
-    <col min="7691" max="7936" width="9.140625" style="25"/>
-    <col min="7937" max="7937" width="6.42578125" style="25" customWidth="1"/>
-    <col min="7938" max="7938" width="11.5703125" style="25" customWidth="1"/>
-    <col min="7939" max="7939" width="39.140625" style="25" customWidth="1"/>
-    <col min="7940" max="7945" width="9.140625" style="25"/>
-    <col min="7946" max="7946" width="10.42578125" style="25" customWidth="1"/>
-    <col min="7947" max="8192" width="9.140625" style="25"/>
-    <col min="8193" max="8193" width="6.42578125" style="25" customWidth="1"/>
-    <col min="8194" max="8194" width="11.5703125" style="25" customWidth="1"/>
-    <col min="8195" max="8195" width="39.140625" style="25" customWidth="1"/>
-    <col min="8196" max="8201" width="9.140625" style="25"/>
-    <col min="8202" max="8202" width="10.42578125" style="25" customWidth="1"/>
-    <col min="8203" max="8448" width="9.140625" style="25"/>
-    <col min="8449" max="8449" width="6.42578125" style="25" customWidth="1"/>
-    <col min="8450" max="8450" width="11.5703125" style="25" customWidth="1"/>
-    <col min="8451" max="8451" width="39.140625" style="25" customWidth="1"/>
-    <col min="8452" max="8457" width="9.140625" style="25"/>
-    <col min="8458" max="8458" width="10.42578125" style="25" customWidth="1"/>
-    <col min="8459" max="8704" width="9.140625" style="25"/>
-    <col min="8705" max="8705" width="6.42578125" style="25" customWidth="1"/>
-    <col min="8706" max="8706" width="11.5703125" style="25" customWidth="1"/>
-    <col min="8707" max="8707" width="39.140625" style="25" customWidth="1"/>
-    <col min="8708" max="8713" width="9.140625" style="25"/>
-    <col min="8714" max="8714" width="10.42578125" style="25" customWidth="1"/>
-    <col min="8715" max="8960" width="9.140625" style="25"/>
-    <col min="8961" max="8961" width="6.42578125" style="25" customWidth="1"/>
-    <col min="8962" max="8962" width="11.5703125" style="25" customWidth="1"/>
-    <col min="8963" max="8963" width="39.140625" style="25" customWidth="1"/>
-    <col min="8964" max="8969" width="9.140625" style="25"/>
-    <col min="8970" max="8970" width="10.42578125" style="25" customWidth="1"/>
-    <col min="8971" max="9216" width="9.140625" style="25"/>
-    <col min="9217" max="9217" width="6.42578125" style="25" customWidth="1"/>
-    <col min="9218" max="9218" width="11.5703125" style="25" customWidth="1"/>
-    <col min="9219" max="9219" width="39.140625" style="25" customWidth="1"/>
-    <col min="9220" max="9225" width="9.140625" style="25"/>
-    <col min="9226" max="9226" width="10.42578125" style="25" customWidth="1"/>
-    <col min="9227" max="9472" width="9.140625" style="25"/>
-    <col min="9473" max="9473" width="6.42578125" style="25" customWidth="1"/>
-    <col min="9474" max="9474" width="11.5703125" style="25" customWidth="1"/>
-    <col min="9475" max="9475" width="39.140625" style="25" customWidth="1"/>
-    <col min="9476" max="9481" width="9.140625" style="25"/>
-    <col min="9482" max="9482" width="10.42578125" style="25" customWidth="1"/>
-    <col min="9483" max="9728" width="9.140625" style="25"/>
-    <col min="9729" max="9729" width="6.42578125" style="25" customWidth="1"/>
-    <col min="9730" max="9730" width="11.5703125" style="25" customWidth="1"/>
-    <col min="9731" max="9731" width="39.140625" style="25" customWidth="1"/>
-    <col min="9732" max="9737" width="9.140625" style="25"/>
-    <col min="9738" max="9738" width="10.42578125" style="25" customWidth="1"/>
-    <col min="9739" max="9984" width="9.140625" style="25"/>
-    <col min="9985" max="9985" width="6.42578125" style="25" customWidth="1"/>
-    <col min="9986" max="9986" width="11.5703125" style="25" customWidth="1"/>
-    <col min="9987" max="9987" width="39.140625" style="25" customWidth="1"/>
-    <col min="9988" max="9993" width="9.140625" style="25"/>
-    <col min="9994" max="9994" width="10.42578125" style="25" customWidth="1"/>
-    <col min="9995" max="10240" width="9.140625" style="25"/>
-    <col min="10241" max="10241" width="6.42578125" style="25" customWidth="1"/>
-    <col min="10242" max="10242" width="11.5703125" style="25" customWidth="1"/>
-    <col min="10243" max="10243" width="39.140625" style="25" customWidth="1"/>
-    <col min="10244" max="10249" width="9.140625" style="25"/>
-    <col min="10250" max="10250" width="10.42578125" style="25" customWidth="1"/>
-    <col min="10251" max="10496" width="9.140625" style="25"/>
-    <col min="10497" max="10497" width="6.42578125" style="25" customWidth="1"/>
-    <col min="10498" max="10498" width="11.5703125" style="25" customWidth="1"/>
-    <col min="10499" max="10499" width="39.140625" style="25" customWidth="1"/>
-    <col min="10500" max="10505" width="9.140625" style="25"/>
-    <col min="10506" max="10506" width="10.42578125" style="25" customWidth="1"/>
-    <col min="10507" max="10752" width="9.140625" style="25"/>
-    <col min="10753" max="10753" width="6.42578125" style="25" customWidth="1"/>
-    <col min="10754" max="10754" width="11.5703125" style="25" customWidth="1"/>
-    <col min="10755" max="10755" width="39.140625" style="25" customWidth="1"/>
-    <col min="10756" max="10761" width="9.140625" style="25"/>
-    <col min="10762" max="10762" width="10.42578125" style="25" customWidth="1"/>
-    <col min="10763" max="11008" width="9.140625" style="25"/>
-    <col min="11009" max="11009" width="6.42578125" style="25" customWidth="1"/>
-    <col min="11010" max="11010" width="11.5703125" style="25" customWidth="1"/>
-    <col min="11011" max="11011" width="39.140625" style="25" customWidth="1"/>
-    <col min="11012" max="11017" width="9.140625" style="25"/>
-    <col min="11018" max="11018" width="10.42578125" style="25" customWidth="1"/>
-    <col min="11019" max="11264" width="9.140625" style="25"/>
-    <col min="11265" max="11265" width="6.42578125" style="25" customWidth="1"/>
-    <col min="11266" max="11266" width="11.5703125" style="25" customWidth="1"/>
-    <col min="11267" max="11267" width="39.140625" style="25" customWidth="1"/>
-    <col min="11268" max="11273" width="9.140625" style="25"/>
-    <col min="11274" max="11274" width="10.42578125" style="25" customWidth="1"/>
-    <col min="11275" max="11520" width="9.140625" style="25"/>
-    <col min="11521" max="11521" width="6.42578125" style="25" customWidth="1"/>
-    <col min="11522" max="11522" width="11.5703125" style="25" customWidth="1"/>
-    <col min="11523" max="11523" width="39.140625" style="25" customWidth="1"/>
-    <col min="11524" max="11529" width="9.140625" style="25"/>
-    <col min="11530" max="11530" width="10.42578125" style="25" customWidth="1"/>
-    <col min="11531" max="11776" width="9.140625" style="25"/>
-    <col min="11777" max="11777" width="6.42578125" style="25" customWidth="1"/>
-    <col min="11778" max="11778" width="11.5703125" style="25" customWidth="1"/>
-    <col min="11779" max="11779" width="39.140625" style="25" customWidth="1"/>
-    <col min="11780" max="11785" width="9.140625" style="25"/>
-    <col min="11786" max="11786" width="10.42578125" style="25" customWidth="1"/>
-    <col min="11787" max="12032" width="9.140625" style="25"/>
-    <col min="12033" max="12033" width="6.42578125" style="25" customWidth="1"/>
-    <col min="12034" max="12034" width="11.5703125" style="25" customWidth="1"/>
-    <col min="12035" max="12035" width="39.140625" style="25" customWidth="1"/>
-    <col min="12036" max="12041" width="9.140625" style="25"/>
-    <col min="12042" max="12042" width="10.42578125" style="25" customWidth="1"/>
-    <col min="12043" max="12288" width="9.140625" style="25"/>
-    <col min="12289" max="12289" width="6.42578125" style="25" customWidth="1"/>
-    <col min="12290" max="12290" width="11.5703125" style="25" customWidth="1"/>
-    <col min="12291" max="12291" width="39.140625" style="25" customWidth="1"/>
-    <col min="12292" max="12297" width="9.140625" style="25"/>
-    <col min="12298" max="12298" width="10.42578125" style="25" customWidth="1"/>
-    <col min="12299" max="12544" width="9.140625" style="25"/>
-    <col min="12545" max="12545" width="6.42578125" style="25" customWidth="1"/>
-    <col min="12546" max="12546" width="11.5703125" style="25" customWidth="1"/>
-    <col min="12547" max="12547" width="39.140625" style="25" customWidth="1"/>
-    <col min="12548" max="12553" width="9.140625" style="25"/>
-    <col min="12554" max="12554" width="10.42578125" style="25" customWidth="1"/>
-    <col min="12555" max="12800" width="9.140625" style="25"/>
-    <col min="12801" max="12801" width="6.42578125" style="25" customWidth="1"/>
-    <col min="12802" max="12802" width="11.5703125" style="25" customWidth="1"/>
-    <col min="12803" max="12803" width="39.140625" style="25" customWidth="1"/>
-    <col min="12804" max="12809" width="9.140625" style="25"/>
-    <col min="12810" max="12810" width="10.42578125" style="25" customWidth="1"/>
-    <col min="12811" max="13056" width="9.140625" style="25"/>
-    <col min="13057" max="13057" width="6.42578125" style="25" customWidth="1"/>
-    <col min="13058" max="13058" width="11.5703125" style="25" customWidth="1"/>
-    <col min="13059" max="13059" width="39.140625" style="25" customWidth="1"/>
-    <col min="13060" max="13065" width="9.140625" style="25"/>
-    <col min="13066" max="13066" width="10.42578125" style="25" customWidth="1"/>
-    <col min="13067" max="13312" width="9.140625" style="25"/>
-    <col min="13313" max="13313" width="6.42578125" style="25" customWidth="1"/>
-    <col min="13314" max="13314" width="11.5703125" style="25" customWidth="1"/>
-    <col min="13315" max="13315" width="39.140625" style="25" customWidth="1"/>
-    <col min="13316" max="13321" width="9.140625" style="25"/>
-    <col min="13322" max="13322" width="10.42578125" style="25" customWidth="1"/>
-    <col min="13323" max="13568" width="9.140625" style="25"/>
-    <col min="13569" max="13569" width="6.42578125" style="25" customWidth="1"/>
-    <col min="13570" max="13570" width="11.5703125" style="25" customWidth="1"/>
-    <col min="13571" max="13571" width="39.140625" style="25" customWidth="1"/>
-    <col min="13572" max="13577" width="9.140625" style="25"/>
-    <col min="13578" max="13578" width="10.42578125" style="25" customWidth="1"/>
-    <col min="13579" max="13824" width="9.140625" style="25"/>
-    <col min="13825" max="13825" width="6.42578125" style="25" customWidth="1"/>
-    <col min="13826" max="13826" width="11.5703125" style="25" customWidth="1"/>
-    <col min="13827" max="13827" width="39.140625" style="25" customWidth="1"/>
-    <col min="13828" max="13833" width="9.140625" style="25"/>
-    <col min="13834" max="13834" width="10.42578125" style="25" customWidth="1"/>
-    <col min="13835" max="14080" width="9.140625" style="25"/>
-    <col min="14081" max="14081" width="6.42578125" style="25" customWidth="1"/>
-    <col min="14082" max="14082" width="11.5703125" style="25" customWidth="1"/>
-    <col min="14083" max="14083" width="39.140625" style="25" customWidth="1"/>
-    <col min="14084" max="14089" width="9.140625" style="25"/>
-    <col min="14090" max="14090" width="10.42578125" style="25" customWidth="1"/>
-    <col min="14091" max="14336" width="9.140625" style="25"/>
-    <col min="14337" max="14337" width="6.42578125" style="25" customWidth="1"/>
-    <col min="14338" max="14338" width="11.5703125" style="25" customWidth="1"/>
-    <col min="14339" max="14339" width="39.140625" style="25" customWidth="1"/>
-    <col min="14340" max="14345" width="9.140625" style="25"/>
-    <col min="14346" max="14346" width="10.42578125" style="25" customWidth="1"/>
-    <col min="14347" max="14592" width="9.140625" style="25"/>
-    <col min="14593" max="14593" width="6.42578125" style="25" customWidth="1"/>
-    <col min="14594" max="14594" width="11.5703125" style="25" customWidth="1"/>
-    <col min="14595" max="14595" width="39.140625" style="25" customWidth="1"/>
-    <col min="14596" max="14601" width="9.140625" style="25"/>
-    <col min="14602" max="14602" width="10.42578125" style="25" customWidth="1"/>
-    <col min="14603" max="14848" width="9.140625" style="25"/>
-    <col min="14849" max="14849" width="6.42578125" style="25" customWidth="1"/>
-    <col min="14850" max="14850" width="11.5703125" style="25" customWidth="1"/>
-    <col min="14851" max="14851" width="39.140625" style="25" customWidth="1"/>
-    <col min="14852" max="14857" width="9.140625" style="25"/>
-    <col min="14858" max="14858" width="10.42578125" style="25" customWidth="1"/>
-    <col min="14859" max="15104" width="9.140625" style="25"/>
-    <col min="15105" max="15105" width="6.42578125" style="25" customWidth="1"/>
-    <col min="15106" max="15106" width="11.5703125" style="25" customWidth="1"/>
-    <col min="15107" max="15107" width="39.140625" style="25" customWidth="1"/>
-    <col min="15108" max="15113" width="9.140625" style="25"/>
-    <col min="15114" max="15114" width="10.42578125" style="25" customWidth="1"/>
-    <col min="15115" max="15360" width="9.140625" style="25"/>
-    <col min="15361" max="15361" width="6.42578125" style="25" customWidth="1"/>
-    <col min="15362" max="15362" width="11.5703125" style="25" customWidth="1"/>
-    <col min="15363" max="15363" width="39.140625" style="25" customWidth="1"/>
-    <col min="15364" max="15369" width="9.140625" style="25"/>
-    <col min="15370" max="15370" width="10.42578125" style="25" customWidth="1"/>
-    <col min="15371" max="15616" width="9.140625" style="25"/>
-    <col min="15617" max="15617" width="6.42578125" style="25" customWidth="1"/>
-    <col min="15618" max="15618" width="11.5703125" style="25" customWidth="1"/>
-    <col min="15619" max="15619" width="39.140625" style="25" customWidth="1"/>
-    <col min="15620" max="15625" width="9.140625" style="25"/>
-    <col min="15626" max="15626" width="10.42578125" style="25" customWidth="1"/>
-    <col min="15627" max="15872" width="9.140625" style="25"/>
-    <col min="15873" max="15873" width="6.42578125" style="25" customWidth="1"/>
-    <col min="15874" max="15874" width="11.5703125" style="25" customWidth="1"/>
-    <col min="15875" max="15875" width="39.140625" style="25" customWidth="1"/>
-    <col min="15876" max="15881" width="9.140625" style="25"/>
-    <col min="15882" max="15882" width="10.42578125" style="25" customWidth="1"/>
-    <col min="15883" max="16128" width="9.140625" style="25"/>
-    <col min="16129" max="16129" width="6.42578125" style="25" customWidth="1"/>
-    <col min="16130" max="16130" width="11.5703125" style="25" customWidth="1"/>
-    <col min="16131" max="16131" width="39.140625" style="25" customWidth="1"/>
-    <col min="16132" max="16137" width="9.140625" style="25"/>
-    <col min="16138" max="16138" width="10.42578125" style="25" customWidth="1"/>
-    <col min="16139" max="16384" width="9.140625" style="25"/>
+    <col min="1" max="1" width="6.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="21"/>
+    <col min="6" max="6" width="5.7109375" style="21" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="21" customWidth="1"/>
+    <col min="9" max="9" width="8" style="21" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="21" customWidth="1"/>
+    <col min="11" max="256" width="9.140625" style="21"/>
+    <col min="257" max="257" width="6.42578125" style="21" customWidth="1"/>
+    <col min="258" max="258" width="11.5703125" style="21" customWidth="1"/>
+    <col min="259" max="259" width="39.140625" style="21" customWidth="1"/>
+    <col min="260" max="265" width="9.140625" style="21"/>
+    <col min="266" max="266" width="10.42578125" style="21" customWidth="1"/>
+    <col min="267" max="512" width="9.140625" style="21"/>
+    <col min="513" max="513" width="6.42578125" style="21" customWidth="1"/>
+    <col min="514" max="514" width="11.5703125" style="21" customWidth="1"/>
+    <col min="515" max="515" width="39.140625" style="21" customWidth="1"/>
+    <col min="516" max="521" width="9.140625" style="21"/>
+    <col min="522" max="522" width="10.42578125" style="21" customWidth="1"/>
+    <col min="523" max="768" width="9.140625" style="21"/>
+    <col min="769" max="769" width="6.42578125" style="21" customWidth="1"/>
+    <col min="770" max="770" width="11.5703125" style="21" customWidth="1"/>
+    <col min="771" max="771" width="39.140625" style="21" customWidth="1"/>
+    <col min="772" max="777" width="9.140625" style="21"/>
+    <col min="778" max="778" width="10.42578125" style="21" customWidth="1"/>
+    <col min="779" max="1024" width="9.140625" style="21"/>
+    <col min="1025" max="1025" width="6.42578125" style="21" customWidth="1"/>
+    <col min="1026" max="1026" width="11.5703125" style="21" customWidth="1"/>
+    <col min="1027" max="1027" width="39.140625" style="21" customWidth="1"/>
+    <col min="1028" max="1033" width="9.140625" style="21"/>
+    <col min="1034" max="1034" width="10.42578125" style="21" customWidth="1"/>
+    <col min="1035" max="1280" width="9.140625" style="21"/>
+    <col min="1281" max="1281" width="6.42578125" style="21" customWidth="1"/>
+    <col min="1282" max="1282" width="11.5703125" style="21" customWidth="1"/>
+    <col min="1283" max="1283" width="39.140625" style="21" customWidth="1"/>
+    <col min="1284" max="1289" width="9.140625" style="21"/>
+    <col min="1290" max="1290" width="10.42578125" style="21" customWidth="1"/>
+    <col min="1291" max="1536" width="9.140625" style="21"/>
+    <col min="1537" max="1537" width="6.42578125" style="21" customWidth="1"/>
+    <col min="1538" max="1538" width="11.5703125" style="21" customWidth="1"/>
+    <col min="1539" max="1539" width="39.140625" style="21" customWidth="1"/>
+    <col min="1540" max="1545" width="9.140625" style="21"/>
+    <col min="1546" max="1546" width="10.42578125" style="21" customWidth="1"/>
+    <col min="1547" max="1792" width="9.140625" style="21"/>
+    <col min="1793" max="1793" width="6.42578125" style="21" customWidth="1"/>
+    <col min="1794" max="1794" width="11.5703125" style="21" customWidth="1"/>
+    <col min="1795" max="1795" width="39.140625" style="21" customWidth="1"/>
+    <col min="1796" max="1801" width="9.140625" style="21"/>
+    <col min="1802" max="1802" width="10.42578125" style="21" customWidth="1"/>
+    <col min="1803" max="2048" width="9.140625" style="21"/>
+    <col min="2049" max="2049" width="6.42578125" style="21" customWidth="1"/>
+    <col min="2050" max="2050" width="11.5703125" style="21" customWidth="1"/>
+    <col min="2051" max="2051" width="39.140625" style="21" customWidth="1"/>
+    <col min="2052" max="2057" width="9.140625" style="21"/>
+    <col min="2058" max="2058" width="10.42578125" style="21" customWidth="1"/>
+    <col min="2059" max="2304" width="9.140625" style="21"/>
+    <col min="2305" max="2305" width="6.42578125" style="21" customWidth="1"/>
+    <col min="2306" max="2306" width="11.5703125" style="21" customWidth="1"/>
+    <col min="2307" max="2307" width="39.140625" style="21" customWidth="1"/>
+    <col min="2308" max="2313" width="9.140625" style="21"/>
+    <col min="2314" max="2314" width="10.42578125" style="21" customWidth="1"/>
+    <col min="2315" max="2560" width="9.140625" style="21"/>
+    <col min="2561" max="2561" width="6.42578125" style="21" customWidth="1"/>
+    <col min="2562" max="2562" width="11.5703125" style="21" customWidth="1"/>
+    <col min="2563" max="2563" width="39.140625" style="21" customWidth="1"/>
+    <col min="2564" max="2569" width="9.140625" style="21"/>
+    <col min="2570" max="2570" width="10.42578125" style="21" customWidth="1"/>
+    <col min="2571" max="2816" width="9.140625" style="21"/>
+    <col min="2817" max="2817" width="6.42578125" style="21" customWidth="1"/>
+    <col min="2818" max="2818" width="11.5703125" style="21" customWidth="1"/>
+    <col min="2819" max="2819" width="39.140625" style="21" customWidth="1"/>
+    <col min="2820" max="2825" width="9.140625" style="21"/>
+    <col min="2826" max="2826" width="10.42578125" style="21" customWidth="1"/>
+    <col min="2827" max="3072" width="9.140625" style="21"/>
+    <col min="3073" max="3073" width="6.42578125" style="21" customWidth="1"/>
+    <col min="3074" max="3074" width="11.5703125" style="21" customWidth="1"/>
+    <col min="3075" max="3075" width="39.140625" style="21" customWidth="1"/>
+    <col min="3076" max="3081" width="9.140625" style="21"/>
+    <col min="3082" max="3082" width="10.42578125" style="21" customWidth="1"/>
+    <col min="3083" max="3328" width="9.140625" style="21"/>
+    <col min="3329" max="3329" width="6.42578125" style="21" customWidth="1"/>
+    <col min="3330" max="3330" width="11.5703125" style="21" customWidth="1"/>
+    <col min="3331" max="3331" width="39.140625" style="21" customWidth="1"/>
+    <col min="3332" max="3337" width="9.140625" style="21"/>
+    <col min="3338" max="3338" width="10.42578125" style="21" customWidth="1"/>
+    <col min="3339" max="3584" width="9.140625" style="21"/>
+    <col min="3585" max="3585" width="6.42578125" style="21" customWidth="1"/>
+    <col min="3586" max="3586" width="11.5703125" style="21" customWidth="1"/>
+    <col min="3587" max="3587" width="39.140625" style="21" customWidth="1"/>
+    <col min="3588" max="3593" width="9.140625" style="21"/>
+    <col min="3594" max="3594" width="10.42578125" style="21" customWidth="1"/>
+    <col min="3595" max="3840" width="9.140625" style="21"/>
+    <col min="3841" max="3841" width="6.42578125" style="21" customWidth="1"/>
+    <col min="3842" max="3842" width="11.5703125" style="21" customWidth="1"/>
+    <col min="3843" max="3843" width="39.140625" style="21" customWidth="1"/>
+    <col min="3844" max="3849" width="9.140625" style="21"/>
+    <col min="3850" max="3850" width="10.42578125" style="21" customWidth="1"/>
+    <col min="3851" max="4096" width="9.140625" style="21"/>
+    <col min="4097" max="4097" width="6.42578125" style="21" customWidth="1"/>
+    <col min="4098" max="4098" width="11.5703125" style="21" customWidth="1"/>
+    <col min="4099" max="4099" width="39.140625" style="21" customWidth="1"/>
+    <col min="4100" max="4105" width="9.140625" style="21"/>
+    <col min="4106" max="4106" width="10.42578125" style="21" customWidth="1"/>
+    <col min="4107" max="4352" width="9.140625" style="21"/>
+    <col min="4353" max="4353" width="6.42578125" style="21" customWidth="1"/>
+    <col min="4354" max="4354" width="11.5703125" style="21" customWidth="1"/>
+    <col min="4355" max="4355" width="39.140625" style="21" customWidth="1"/>
+    <col min="4356" max="4361" width="9.140625" style="21"/>
+    <col min="4362" max="4362" width="10.42578125" style="21" customWidth="1"/>
+    <col min="4363" max="4608" width="9.140625" style="21"/>
+    <col min="4609" max="4609" width="6.42578125" style="21" customWidth="1"/>
+    <col min="4610" max="4610" width="11.5703125" style="21" customWidth="1"/>
+    <col min="4611" max="4611" width="39.140625" style="21" customWidth="1"/>
+    <col min="4612" max="4617" width="9.140625" style="21"/>
+    <col min="4618" max="4618" width="10.42578125" style="21" customWidth="1"/>
+    <col min="4619" max="4864" width="9.140625" style="21"/>
+    <col min="4865" max="4865" width="6.42578125" style="21" customWidth="1"/>
+    <col min="4866" max="4866" width="11.5703125" style="21" customWidth="1"/>
+    <col min="4867" max="4867" width="39.140625" style="21" customWidth="1"/>
+    <col min="4868" max="4873" width="9.140625" style="21"/>
+    <col min="4874" max="4874" width="10.42578125" style="21" customWidth="1"/>
+    <col min="4875" max="5120" width="9.140625" style="21"/>
+    <col min="5121" max="5121" width="6.42578125" style="21" customWidth="1"/>
+    <col min="5122" max="5122" width="11.5703125" style="21" customWidth="1"/>
+    <col min="5123" max="5123" width="39.140625" style="21" customWidth="1"/>
+    <col min="5124" max="5129" width="9.140625" style="21"/>
+    <col min="5130" max="5130" width="10.42578125" style="21" customWidth="1"/>
+    <col min="5131" max="5376" width="9.140625" style="21"/>
+    <col min="5377" max="5377" width="6.42578125" style="21" customWidth="1"/>
+    <col min="5378" max="5378" width="11.5703125" style="21" customWidth="1"/>
+    <col min="5379" max="5379" width="39.140625" style="21" customWidth="1"/>
+    <col min="5380" max="5385" width="9.140625" style="21"/>
+    <col min="5386" max="5386" width="10.42578125" style="21" customWidth="1"/>
+    <col min="5387" max="5632" width="9.140625" style="21"/>
+    <col min="5633" max="5633" width="6.42578125" style="21" customWidth="1"/>
+    <col min="5634" max="5634" width="11.5703125" style="21" customWidth="1"/>
+    <col min="5635" max="5635" width="39.140625" style="21" customWidth="1"/>
+    <col min="5636" max="5641" width="9.140625" style="21"/>
+    <col min="5642" max="5642" width="10.42578125" style="21" customWidth="1"/>
+    <col min="5643" max="5888" width="9.140625" style="21"/>
+    <col min="5889" max="5889" width="6.42578125" style="21" customWidth="1"/>
+    <col min="5890" max="5890" width="11.5703125" style="21" customWidth="1"/>
+    <col min="5891" max="5891" width="39.140625" style="21" customWidth="1"/>
+    <col min="5892" max="5897" width="9.140625" style="21"/>
+    <col min="5898" max="5898" width="10.42578125" style="21" customWidth="1"/>
+    <col min="5899" max="6144" width="9.140625" style="21"/>
+    <col min="6145" max="6145" width="6.42578125" style="21" customWidth="1"/>
+    <col min="6146" max="6146" width="11.5703125" style="21" customWidth="1"/>
+    <col min="6147" max="6147" width="39.140625" style="21" customWidth="1"/>
+    <col min="6148" max="6153" width="9.140625" style="21"/>
+    <col min="6154" max="6154" width="10.42578125" style="21" customWidth="1"/>
+    <col min="6155" max="6400" width="9.140625" style="21"/>
+    <col min="6401" max="6401" width="6.42578125" style="21" customWidth="1"/>
+    <col min="6402" max="6402" width="11.5703125" style="21" customWidth="1"/>
+    <col min="6403" max="6403" width="39.140625" style="21" customWidth="1"/>
+    <col min="6404" max="6409" width="9.140625" style="21"/>
+    <col min="6410" max="6410" width="10.42578125" style="21" customWidth="1"/>
+    <col min="6411" max="6656" width="9.140625" style="21"/>
+    <col min="6657" max="6657" width="6.42578125" style="21" customWidth="1"/>
+    <col min="6658" max="6658" width="11.5703125" style="21" customWidth="1"/>
+    <col min="6659" max="6659" width="39.140625" style="21" customWidth="1"/>
+    <col min="6660" max="6665" width="9.140625" style="21"/>
+    <col min="6666" max="6666" width="10.42578125" style="21" customWidth="1"/>
+    <col min="6667" max="6912" width="9.140625" style="21"/>
+    <col min="6913" max="6913" width="6.42578125" style="21" customWidth="1"/>
+    <col min="6914" max="6914" width="11.5703125" style="21" customWidth="1"/>
+    <col min="6915" max="6915" width="39.140625" style="21" customWidth="1"/>
+    <col min="6916" max="6921" width="9.140625" style="21"/>
+    <col min="6922" max="6922" width="10.42578125" style="21" customWidth="1"/>
+    <col min="6923" max="7168" width="9.140625" style="21"/>
+    <col min="7169" max="7169" width="6.42578125" style="21" customWidth="1"/>
+    <col min="7170" max="7170" width="11.5703125" style="21" customWidth="1"/>
+    <col min="7171" max="7171" width="39.140625" style="21" customWidth="1"/>
+    <col min="7172" max="7177" width="9.140625" style="21"/>
+    <col min="7178" max="7178" width="10.42578125" style="21" customWidth="1"/>
+    <col min="7179" max="7424" width="9.140625" style="21"/>
+    <col min="7425" max="7425" width="6.42578125" style="21" customWidth="1"/>
+    <col min="7426" max="7426" width="11.5703125" style="21" customWidth="1"/>
+    <col min="7427" max="7427" width="39.140625" style="21" customWidth="1"/>
+    <col min="7428" max="7433" width="9.140625" style="21"/>
+    <col min="7434" max="7434" width="10.42578125" style="21" customWidth="1"/>
+    <col min="7435" max="7680" width="9.140625" style="21"/>
+    <col min="7681" max="7681" width="6.42578125" style="21" customWidth="1"/>
+    <col min="7682" max="7682" width="11.5703125" style="21" customWidth="1"/>
+    <col min="7683" max="7683" width="39.140625" style="21" customWidth="1"/>
+    <col min="7684" max="7689" width="9.140625" style="21"/>
+    <col min="7690" max="7690" width="10.42578125" style="21" customWidth="1"/>
+    <col min="7691" max="7936" width="9.140625" style="21"/>
+    <col min="7937" max="7937" width="6.42578125" style="21" customWidth="1"/>
+    <col min="7938" max="7938" width="11.5703125" style="21" customWidth="1"/>
+    <col min="7939" max="7939" width="39.140625" style="21" customWidth="1"/>
+    <col min="7940" max="7945" width="9.140625" style="21"/>
+    <col min="7946" max="7946" width="10.42578125" style="21" customWidth="1"/>
+    <col min="7947" max="8192" width="9.140625" style="21"/>
+    <col min="8193" max="8193" width="6.42578125" style="21" customWidth="1"/>
+    <col min="8194" max="8194" width="11.5703125" style="21" customWidth="1"/>
+    <col min="8195" max="8195" width="39.140625" style="21" customWidth="1"/>
+    <col min="8196" max="8201" width="9.140625" style="21"/>
+    <col min="8202" max="8202" width="10.42578125" style="21" customWidth="1"/>
+    <col min="8203" max="8448" width="9.140625" style="21"/>
+    <col min="8449" max="8449" width="6.42578125" style="21" customWidth="1"/>
+    <col min="8450" max="8450" width="11.5703125" style="21" customWidth="1"/>
+    <col min="8451" max="8451" width="39.140625" style="21" customWidth="1"/>
+    <col min="8452" max="8457" width="9.140625" style="21"/>
+    <col min="8458" max="8458" width="10.42578125" style="21" customWidth="1"/>
+    <col min="8459" max="8704" width="9.140625" style="21"/>
+    <col min="8705" max="8705" width="6.42578125" style="21" customWidth="1"/>
+    <col min="8706" max="8706" width="11.5703125" style="21" customWidth="1"/>
+    <col min="8707" max="8707" width="39.140625" style="21" customWidth="1"/>
+    <col min="8708" max="8713" width="9.140625" style="21"/>
+    <col min="8714" max="8714" width="10.42578125" style="21" customWidth="1"/>
+    <col min="8715" max="8960" width="9.140625" style="21"/>
+    <col min="8961" max="8961" width="6.42578125" style="21" customWidth="1"/>
+    <col min="8962" max="8962" width="11.5703125" style="21" customWidth="1"/>
+    <col min="8963" max="8963" width="39.140625" style="21" customWidth="1"/>
+    <col min="8964" max="8969" width="9.140625" style="21"/>
+    <col min="8970" max="8970" width="10.42578125" style="21" customWidth="1"/>
+    <col min="8971" max="9216" width="9.140625" style="21"/>
+    <col min="9217" max="9217" width="6.42578125" style="21" customWidth="1"/>
+    <col min="9218" max="9218" width="11.5703125" style="21" customWidth="1"/>
+    <col min="9219" max="9219" width="39.140625" style="21" customWidth="1"/>
+    <col min="9220" max="9225" width="9.140625" style="21"/>
+    <col min="9226" max="9226" width="10.42578125" style="21" customWidth="1"/>
+    <col min="9227" max="9472" width="9.140625" style="21"/>
+    <col min="9473" max="9473" width="6.42578125" style="21" customWidth="1"/>
+    <col min="9474" max="9474" width="11.5703125" style="21" customWidth="1"/>
+    <col min="9475" max="9475" width="39.140625" style="21" customWidth="1"/>
+    <col min="9476" max="9481" width="9.140625" style="21"/>
+    <col min="9482" max="9482" width="10.42578125" style="21" customWidth="1"/>
+    <col min="9483" max="9728" width="9.140625" style="21"/>
+    <col min="9729" max="9729" width="6.42578125" style="21" customWidth="1"/>
+    <col min="9730" max="9730" width="11.5703125" style="21" customWidth="1"/>
+    <col min="9731" max="9731" width="39.140625" style="21" customWidth="1"/>
+    <col min="9732" max="9737" width="9.140625" style="21"/>
+    <col min="9738" max="9738" width="10.42578125" style="21" customWidth="1"/>
+    <col min="9739" max="9984" width="9.140625" style="21"/>
+    <col min="9985" max="9985" width="6.42578125" style="21" customWidth="1"/>
+    <col min="9986" max="9986" width="11.5703125" style="21" customWidth="1"/>
+    <col min="9987" max="9987" width="39.140625" style="21" customWidth="1"/>
+    <col min="9988" max="9993" width="9.140625" style="21"/>
+    <col min="9994" max="9994" width="10.42578125" style="21" customWidth="1"/>
+    <col min="9995" max="10240" width="9.140625" style="21"/>
+    <col min="10241" max="10241" width="6.42578125" style="21" customWidth="1"/>
+    <col min="10242" max="10242" width="11.5703125" style="21" customWidth="1"/>
+    <col min="10243" max="10243" width="39.140625" style="21" customWidth="1"/>
+    <col min="10244" max="10249" width="9.140625" style="21"/>
+    <col min="10250" max="10250" width="10.42578125" style="21" customWidth="1"/>
+    <col min="10251" max="10496" width="9.140625" style="21"/>
+    <col min="10497" max="10497" width="6.42578125" style="21" customWidth="1"/>
+    <col min="10498" max="10498" width="11.5703125" style="21" customWidth="1"/>
+    <col min="10499" max="10499" width="39.140625" style="21" customWidth="1"/>
+    <col min="10500" max="10505" width="9.140625" style="21"/>
+    <col min="10506" max="10506" width="10.42578125" style="21" customWidth="1"/>
+    <col min="10507" max="10752" width="9.140625" style="21"/>
+    <col min="10753" max="10753" width="6.42578125" style="21" customWidth="1"/>
+    <col min="10754" max="10754" width="11.5703125" style="21" customWidth="1"/>
+    <col min="10755" max="10755" width="39.140625" style="21" customWidth="1"/>
+    <col min="10756" max="10761" width="9.140625" style="21"/>
+    <col min="10762" max="10762" width="10.42578125" style="21" customWidth="1"/>
+    <col min="10763" max="11008" width="9.140625" style="21"/>
+    <col min="11009" max="11009" width="6.42578125" style="21" customWidth="1"/>
+    <col min="11010" max="11010" width="11.5703125" style="21" customWidth="1"/>
+    <col min="11011" max="11011" width="39.140625" style="21" customWidth="1"/>
+    <col min="11012" max="11017" width="9.140625" style="21"/>
+    <col min="11018" max="11018" width="10.42578125" style="21" customWidth="1"/>
+    <col min="11019" max="11264" width="9.140625" style="21"/>
+    <col min="11265" max="11265" width="6.42578125" style="21" customWidth="1"/>
+    <col min="11266" max="11266" width="11.5703125" style="21" customWidth="1"/>
+    <col min="11267" max="11267" width="39.140625" style="21" customWidth="1"/>
+    <col min="11268" max="11273" width="9.140625" style="21"/>
+    <col min="11274" max="11274" width="10.42578125" style="21" customWidth="1"/>
+    <col min="11275" max="11520" width="9.140625" style="21"/>
+    <col min="11521" max="11521" width="6.42578125" style="21" customWidth="1"/>
+    <col min="11522" max="11522" width="11.5703125" style="21" customWidth="1"/>
+    <col min="11523" max="11523" width="39.140625" style="21" customWidth="1"/>
+    <col min="11524" max="11529" width="9.140625" style="21"/>
+    <col min="11530" max="11530" width="10.42578125" style="21" customWidth="1"/>
+    <col min="11531" max="11776" width="9.140625" style="21"/>
+    <col min="11777" max="11777" width="6.42578125" style="21" customWidth="1"/>
+    <col min="11778" max="11778" width="11.5703125" style="21" customWidth="1"/>
+    <col min="11779" max="11779" width="39.140625" style="21" customWidth="1"/>
+    <col min="11780" max="11785" width="9.140625" style="21"/>
+    <col min="11786" max="11786" width="10.42578125" style="21" customWidth="1"/>
+    <col min="11787" max="12032" width="9.140625" style="21"/>
+    <col min="12033" max="12033" width="6.42578125" style="21" customWidth="1"/>
+    <col min="12034" max="12034" width="11.5703125" style="21" customWidth="1"/>
+    <col min="12035" max="12035" width="39.140625" style="21" customWidth="1"/>
+    <col min="12036" max="12041" width="9.140625" style="21"/>
+    <col min="12042" max="12042" width="10.42578125" style="21" customWidth="1"/>
+    <col min="12043" max="12288" width="9.140625" style="21"/>
+    <col min="12289" max="12289" width="6.42578125" style="21" customWidth="1"/>
+    <col min="12290" max="12290" width="11.5703125" style="21" customWidth="1"/>
+    <col min="12291" max="12291" width="39.140625" style="21" customWidth="1"/>
+    <col min="12292" max="12297" width="9.140625" style="21"/>
+    <col min="12298" max="12298" width="10.42578125" style="21" customWidth="1"/>
+    <col min="12299" max="12544" width="9.140625" style="21"/>
+    <col min="12545" max="12545" width="6.42578125" style="21" customWidth="1"/>
+    <col min="12546" max="12546" width="11.5703125" style="21" customWidth="1"/>
+    <col min="12547" max="12547" width="39.140625" style="21" customWidth="1"/>
+    <col min="12548" max="12553" width="9.140625" style="21"/>
+    <col min="12554" max="12554" width="10.42578125" style="21" customWidth="1"/>
+    <col min="12555" max="12800" width="9.140625" style="21"/>
+    <col min="12801" max="12801" width="6.42578125" style="21" customWidth="1"/>
+    <col min="12802" max="12802" width="11.5703125" style="21" customWidth="1"/>
+    <col min="12803" max="12803" width="39.140625" style="21" customWidth="1"/>
+    <col min="12804" max="12809" width="9.140625" style="21"/>
+    <col min="12810" max="12810" width="10.42578125" style="21" customWidth="1"/>
+    <col min="12811" max="13056" width="9.140625" style="21"/>
+    <col min="13057" max="13057" width="6.42578125" style="21" customWidth="1"/>
+    <col min="13058" max="13058" width="11.5703125" style="21" customWidth="1"/>
+    <col min="13059" max="13059" width="39.140625" style="21" customWidth="1"/>
+    <col min="13060" max="13065" width="9.140625" style="21"/>
+    <col min="13066" max="13066" width="10.42578125" style="21" customWidth="1"/>
+    <col min="13067" max="13312" width="9.140625" style="21"/>
+    <col min="13313" max="13313" width="6.42578125" style="21" customWidth="1"/>
+    <col min="13314" max="13314" width="11.5703125" style="21" customWidth="1"/>
+    <col min="13315" max="13315" width="39.140625" style="21" customWidth="1"/>
+    <col min="13316" max="13321" width="9.140625" style="21"/>
+    <col min="13322" max="13322" width="10.42578125" style="21" customWidth="1"/>
+    <col min="13323" max="13568" width="9.140625" style="21"/>
+    <col min="13569" max="13569" width="6.42578125" style="21" customWidth="1"/>
+    <col min="13570" max="13570" width="11.5703125" style="21" customWidth="1"/>
+    <col min="13571" max="13571" width="39.140625" style="21" customWidth="1"/>
+    <col min="13572" max="13577" width="9.140625" style="21"/>
+    <col min="13578" max="13578" width="10.42578125" style="21" customWidth="1"/>
+    <col min="13579" max="13824" width="9.140625" style="21"/>
+    <col min="13825" max="13825" width="6.42578125" style="21" customWidth="1"/>
+    <col min="13826" max="13826" width="11.5703125" style="21" customWidth="1"/>
+    <col min="13827" max="13827" width="39.140625" style="21" customWidth="1"/>
+    <col min="13828" max="13833" width="9.140625" style="21"/>
+    <col min="13834" max="13834" width="10.42578125" style="21" customWidth="1"/>
+    <col min="13835" max="14080" width="9.140625" style="21"/>
+    <col min="14081" max="14081" width="6.42578125" style="21" customWidth="1"/>
+    <col min="14082" max="14082" width="11.5703125" style="21" customWidth="1"/>
+    <col min="14083" max="14083" width="39.140625" style="21" customWidth="1"/>
+    <col min="14084" max="14089" width="9.140625" style="21"/>
+    <col min="14090" max="14090" width="10.42578125" style="21" customWidth="1"/>
+    <col min="14091" max="14336" width="9.140625" style="21"/>
+    <col min="14337" max="14337" width="6.42578125" style="21" customWidth="1"/>
+    <col min="14338" max="14338" width="11.5703125" style="21" customWidth="1"/>
+    <col min="14339" max="14339" width="39.140625" style="21" customWidth="1"/>
+    <col min="14340" max="14345" width="9.140625" style="21"/>
+    <col min="14346" max="14346" width="10.42578125" style="21" customWidth="1"/>
+    <col min="14347" max="14592" width="9.140625" style="21"/>
+    <col min="14593" max="14593" width="6.42578125" style="21" customWidth="1"/>
+    <col min="14594" max="14594" width="11.5703125" style="21" customWidth="1"/>
+    <col min="14595" max="14595" width="39.140625" style="21" customWidth="1"/>
+    <col min="14596" max="14601" width="9.140625" style="21"/>
+    <col min="14602" max="14602" width="10.42578125" style="21" customWidth="1"/>
+    <col min="14603" max="14848" width="9.140625" style="21"/>
+    <col min="14849" max="14849" width="6.42578125" style="21" customWidth="1"/>
+    <col min="14850" max="14850" width="11.5703125" style="21" customWidth="1"/>
+    <col min="14851" max="14851" width="39.140625" style="21" customWidth="1"/>
+    <col min="14852" max="14857" width="9.140625" style="21"/>
+    <col min="14858" max="14858" width="10.42578125" style="21" customWidth="1"/>
+    <col min="14859" max="15104" width="9.140625" style="21"/>
+    <col min="15105" max="15105" width="6.42578125" style="21" customWidth="1"/>
+    <col min="15106" max="15106" width="11.5703125" style="21" customWidth="1"/>
+    <col min="15107" max="15107" width="39.140625" style="21" customWidth="1"/>
+    <col min="15108" max="15113" width="9.140625" style="21"/>
+    <col min="15114" max="15114" width="10.42578125" style="21" customWidth="1"/>
+    <col min="15115" max="15360" width="9.140625" style="21"/>
+    <col min="15361" max="15361" width="6.42578125" style="21" customWidth="1"/>
+    <col min="15362" max="15362" width="11.5703125" style="21" customWidth="1"/>
+    <col min="15363" max="15363" width="39.140625" style="21" customWidth="1"/>
+    <col min="15364" max="15369" width="9.140625" style="21"/>
+    <col min="15370" max="15370" width="10.42578125" style="21" customWidth="1"/>
+    <col min="15371" max="15616" width="9.140625" style="21"/>
+    <col min="15617" max="15617" width="6.42578125" style="21" customWidth="1"/>
+    <col min="15618" max="15618" width="11.5703125" style="21" customWidth="1"/>
+    <col min="15619" max="15619" width="39.140625" style="21" customWidth="1"/>
+    <col min="15620" max="15625" width="9.140625" style="21"/>
+    <col min="15626" max="15626" width="10.42578125" style="21" customWidth="1"/>
+    <col min="15627" max="15872" width="9.140625" style="21"/>
+    <col min="15873" max="15873" width="6.42578125" style="21" customWidth="1"/>
+    <col min="15874" max="15874" width="11.5703125" style="21" customWidth="1"/>
+    <col min="15875" max="15875" width="39.140625" style="21" customWidth="1"/>
+    <col min="15876" max="15881" width="9.140625" style="21"/>
+    <col min="15882" max="15882" width="10.42578125" style="21" customWidth="1"/>
+    <col min="15883" max="16128" width="9.140625" style="21"/>
+    <col min="16129" max="16129" width="6.42578125" style="21" customWidth="1"/>
+    <col min="16130" max="16130" width="11.5703125" style="21" customWidth="1"/>
+    <col min="16131" max="16131" width="39.140625" style="21" customWidth="1"/>
+    <col min="16132" max="16137" width="9.140625" style="21"/>
+    <col min="16138" max="16138" width="10.42578125" style="21" customWidth="1"/>
+    <col min="16139" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
     </row>
     <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="E2" s="24" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="E2" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
     </row>
     <row r="4" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
     </row>
     <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+    </row>
+    <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-    </row>
-    <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-    </row>
-    <row r="7" spans="1:16" s="32" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-    </row>
-    <row r="8" spans="1:16" s="32" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+    </row>
+    <row r="7" spans="1:16" s="25" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+    </row>
+    <row r="8" spans="1:16" s="25" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-    </row>
-    <row r="9" spans="1:16" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:16" s="32" customFormat="1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+    </row>
+    <row r="9" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:16" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="G10" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="H10" s="34" t="s">
+      <c r="H10" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="J10" s="34" t="s">
+      <c r="J10" s="26" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="35">
+    <row r="11" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="27">
         <v>1</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="38">
-        <v>3</v>
-      </c>
-      <c r="E11" s="35" t="s">
+      <c r="D11" s="30">
+        <v>3</v>
+      </c>
+      <c r="E11" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="36">
+      <c r="F11" s="27"/>
+      <c r="G11" s="28">
         <v>45</v>
       </c>
-      <c r="H11" s="36">
+      <c r="H11" s="28">
         <v>30</v>
       </c>
-      <c r="I11" s="36">
+      <c r="I11" s="28">
         <v>12</v>
       </c>
-      <c r="J11" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="35">
+      <c r="J11" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="27">
         <v>2</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="30">
         <v>1</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36">
+      <c r="F12" s="27"/>
+      <c r="G12" s="28">
         <v>30</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="28">
         <v>2</v>
       </c>
-      <c r="I12" s="36">
+      <c r="I12" s="28">
         <v>26</v>
       </c>
-      <c r="J12" s="36">
+      <c r="J12" s="28">
         <v>2</v>
       </c>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-    </row>
-    <row r="13" spans="1:16" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="35">
-        <v>3</v>
-      </c>
-      <c r="B13" s="36" t="s">
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+    </row>
+    <row r="13" spans="1:16" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="27">
+        <v>3</v>
+      </c>
+      <c r="B13" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="38">
-        <v>3</v>
-      </c>
-      <c r="E13" s="35" t="s">
+      <c r="D13" s="30">
+        <v>3</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F13" s="35"/>
-      <c r="G13" s="36">
+      <c r="F13" s="27"/>
+      <c r="G13" s="28">
         <v>45</v>
       </c>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-    </row>
-    <row r="14" spans="1:16" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="35">
-        <v>4</v>
-      </c>
-      <c r="B14" s="36" t="s">
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+    </row>
+    <row r="14" spans="1:16" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="27">
+        <v>4</v>
+      </c>
+      <c r="B14" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="D14" s="38">
-        <v>3</v>
-      </c>
-      <c r="E14" s="35" t="s">
+      <c r="D14" s="30">
+        <v>3</v>
+      </c>
+      <c r="E14" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36">
+      <c r="F14" s="27"/>
+      <c r="G14" s="28">
         <v>60</v>
       </c>
-      <c r="H14" s="36">
+      <c r="H14" s="28">
         <v>30</v>
       </c>
-      <c r="I14" s="36">
+      <c r="I14" s="28">
         <v>25</v>
       </c>
-      <c r="J14" s="36">
+      <c r="J14" s="28">
         <v>5</v>
       </c>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="39"/>
-    </row>
-    <row r="15" spans="1:16" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="35">
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="31"/>
+    </row>
+    <row r="15" spans="1:16" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A15" s="27">
         <v>5</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D15" s="28">
         <v>2</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F15" s="35"/>
-      <c r="G15" s="36">
+      <c r="F15" s="27"/>
+      <c r="G15" s="28">
         <v>45</v>
       </c>
-      <c r="H15" s="36">
+      <c r="H15" s="28">
         <v>17</v>
       </c>
-      <c r="I15" s="36">
+      <c r="I15" s="28">
         <v>25</v>
       </c>
-      <c r="J15" s="36">
-        <v>3</v>
-      </c>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-    </row>
-    <row r="16" spans="1:16" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="35">
+      <c r="J15" s="28">
+        <v>3</v>
+      </c>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+    </row>
+    <row r="16" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="27">
         <v>6</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="38">
-        <v>3</v>
-      </c>
-      <c r="E16" s="35" t="s">
+      <c r="D16" s="30">
+        <v>3</v>
+      </c>
+      <c r="E16" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F16" s="35"/>
-      <c r="G16" s="36">
+      <c r="F16" s="27"/>
+      <c r="G16" s="28">
         <v>75</v>
       </c>
-      <c r="H16" s="36">
+      <c r="H16" s="28">
         <v>17</v>
       </c>
-      <c r="I16" s="36">
+      <c r="I16" s="28">
         <v>54</v>
       </c>
-      <c r="J16" s="36">
-        <v>4</v>
-      </c>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-    </row>
-    <row r="17" spans="1:16" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="35">
+      <c r="J16" s="28">
+        <v>4</v>
+      </c>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+    </row>
+    <row r="17" spans="1:16" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="27">
         <v>7</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="36">
-        <v>3</v>
-      </c>
-      <c r="E17" s="35" t="s">
+      <c r="D17" s="28">
+        <v>3</v>
+      </c>
+      <c r="E17" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F17" s="35"/>
-      <c r="G17" s="36">
+      <c r="F17" s="27"/>
+      <c r="G17" s="28">
         <v>75</v>
       </c>
-      <c r="H17" s="36">
+      <c r="H17" s="28">
         <v>20</v>
       </c>
-      <c r="I17" s="36">
+      <c r="I17" s="28">
         <v>51</v>
       </c>
-      <c r="J17" s="36">
-        <v>4</v>
-      </c>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-    </row>
-    <row r="18" spans="1:16" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="35">
+      <c r="J17" s="28">
+        <v>4</v>
+      </c>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+    </row>
+    <row r="18" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="27">
         <v>8</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="36">
-        <v>3</v>
-      </c>
-      <c r="E18" s="35" t="s">
+      <c r="D18" s="28">
+        <v>3</v>
+      </c>
+      <c r="E18" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F18" s="41"/>
-      <c r="G18" s="36">
+      <c r="F18" s="33"/>
+      <c r="G18" s="28">
         <v>75</v>
       </c>
-      <c r="H18" s="36">
+      <c r="H18" s="28">
         <v>20</v>
       </c>
-      <c r="I18" s="36">
+      <c r="I18" s="28">
         <v>51</v>
       </c>
-      <c r="J18" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="35">
+      <c r="J18" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="27">
         <v>9</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="42">
+      <c r="C19" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="34">
         <v>2</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F19" s="35"/>
-      <c r="G19" s="36">
+      <c r="F19" s="27"/>
+      <c r="G19" s="28">
         <v>30</v>
       </c>
-      <c r="H19" s="36">
+      <c r="H19" s="28">
         <v>21</v>
       </c>
-      <c r="I19" s="36">
+      <c r="I19" s="28">
         <v>7</v>
       </c>
-      <c r="J19" s="36">
+      <c r="J19" s="28">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
+    <row r="20" spans="1:16" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="44">
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="35">
         <f>SUM(D11:D19)</f>
         <v>23</v>
       </c>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44">
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35">
         <f>SUM(G11:G19)</f>
         <v>480</v>
       </c>
-      <c r="H20" s="44">
+      <c r="H20" s="35">
         <f>SUM(H11:H19)</f>
         <v>157</v>
       </c>
-      <c r="I20" s="44">
+      <c r="I20" s="35">
         <f>SUM(I11:I19)</f>
         <v>251</v>
       </c>
-      <c r="J20" s="44">
+      <c r="J20" s="35">
         <f>SUM(J11:J19)</f>
         <v>27</v>
       </c>
-      <c r="K20" s="45"/>
-      <c r="L20" s="39"/>
-    </row>
-    <row r="21" spans="1:16" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:16" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:16" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="33" t="s">
+      <c r="K20" s="36"/>
+      <c r="L20" s="31"/>
+    </row>
+    <row r="21" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:16" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="53" t="s">
         <v>137</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-    </row>
-    <row r="24" spans="1:16" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:16" s="32" customFormat="1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A25" s="34" t="s">
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+    </row>
+    <row r="24" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:16" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+      <c r="A25" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="F25" s="34" t="s">
+      <c r="F25" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="G25" s="34" t="s">
+      <c r="G25" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="H25" s="34" t="s">
+      <c r="H25" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I25" s="34" t="s">
+      <c r="I25" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="J25" s="34" t="s">
+      <c r="J25" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="L25" s="32">
+      <c r="L25" s="25">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="34">
+    <row r="26" spans="1:16" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="26">
         <v>1</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="38">
+      <c r="D26" s="30">
         <v>2</v>
       </c>
-      <c r="E26" s="35" t="s">
+      <c r="E26" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F26" s="35"/>
-      <c r="G26" s="36">
+      <c r="F26" s="27"/>
+      <c r="G26" s="28">
         <v>45</v>
       </c>
-      <c r="H26" s="36">
+      <c r="H26" s="28">
         <v>30</v>
       </c>
-      <c r="I26" s="36">
+      <c r="I26" s="28">
         <v>12</v>
       </c>
-      <c r="J26" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="34">
+      <c r="J26" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="26">
         <v>2</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="D27" s="38">
+      <c r="D27" s="30">
         <v>1</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E27" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="35"/>
-      <c r="G27" s="36">
+      <c r="F27" s="27"/>
+      <c r="G27" s="28">
         <v>30</v>
       </c>
-      <c r="H27" s="36">
+      <c r="H27" s="28">
         <v>2</v>
       </c>
-      <c r="I27" s="36">
+      <c r="I27" s="28">
         <v>26</v>
       </c>
-      <c r="J27" s="36">
+      <c r="J27" s="28">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A28" s="34">
-        <v>3</v>
-      </c>
-      <c r="B28" s="36" t="s">
+    <row r="28" spans="1:16" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A28" s="26">
+        <v>3</v>
+      </c>
+      <c r="B28" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="D28" s="38">
-        <v>3</v>
-      </c>
-      <c r="E28" s="35" t="s">
+      <c r="D28" s="30">
+        <v>3</v>
+      </c>
+      <c r="E28" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F28" s="35"/>
-      <c r="G28" s="36">
+      <c r="F28" s="27"/>
+      <c r="G28" s="28">
         <v>60</v>
       </c>
-      <c r="H28" s="36">
+      <c r="H28" s="28">
         <v>30</v>
       </c>
-      <c r="I28" s="36">
+      <c r="I28" s="28">
         <v>25</v>
       </c>
-      <c r="J28" s="36">
+      <c r="J28" s="28">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" s="34">
-        <v>4</v>
-      </c>
-      <c r="B29" s="36" t="s">
+    <row r="29" spans="1:16" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A29" s="26">
+        <v>4</v>
+      </c>
+      <c r="B29" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D29" s="38">
+      <c r="D29" s="30">
         <v>2</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F29" s="35"/>
-      <c r="G29" s="36">
+      <c r="F29" s="27"/>
+      <c r="G29" s="28">
         <v>30</v>
       </c>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
-    </row>
-    <row r="30" spans="1:16" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="34">
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+    </row>
+    <row r="30" spans="1:16" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="26">
         <v>5</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="36">
-        <v>3</v>
-      </c>
-      <c r="E30" s="35" t="s">
+      <c r="D30" s="28">
+        <v>3</v>
+      </c>
+      <c r="E30" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F30" s="35"/>
-      <c r="G30" s="36">
+      <c r="F30" s="27"/>
+      <c r="G30" s="28">
         <v>75</v>
       </c>
-      <c r="H30" s="36">
+      <c r="H30" s="28">
         <v>20</v>
       </c>
-      <c r="I30" s="36">
+      <c r="I30" s="28">
         <v>51</v>
       </c>
-      <c r="J30" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="34">
+      <c r="J30" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="26">
         <v>6</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="37" t="s">
+      <c r="C31" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="36">
+      <c r="D31" s="28">
         <v>2</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F31" s="35"/>
-      <c r="G31" s="36">
+      <c r="F31" s="27"/>
+      <c r="G31" s="28">
         <v>45</v>
       </c>
-      <c r="H31" s="36">
+      <c r="H31" s="28">
         <v>17</v>
       </c>
-      <c r="I31" s="36">
+      <c r="I31" s="28">
         <v>25</v>
       </c>
-      <c r="J31" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="34">
+      <c r="J31" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="26">
         <v>7</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="36">
-        <v>3</v>
-      </c>
-      <c r="E32" s="35" t="s">
+      <c r="D32" s="28">
+        <v>3</v>
+      </c>
+      <c r="E32" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F32" s="35"/>
-      <c r="G32" s="36">
+      <c r="F32" s="27"/>
+      <c r="G32" s="28">
         <v>75</v>
       </c>
-      <c r="H32" s="36">
+      <c r="H32" s="28">
         <v>20</v>
       </c>
-      <c r="I32" s="36">
+      <c r="I32" s="28">
         <v>51</v>
       </c>
-      <c r="J32" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="34">
+      <c r="J32" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="26">
         <v>8</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="37" t="s">
+      <c r="C33" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="36">
-        <v>3</v>
-      </c>
-      <c r="E33" s="35" t="s">
+      <c r="D33" s="28">
+        <v>3</v>
+      </c>
+      <c r="E33" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F33" s="35"/>
-      <c r="G33" s="36">
+      <c r="F33" s="27"/>
+      <c r="G33" s="28">
         <v>75</v>
       </c>
-      <c r="H33" s="36">
+      <c r="H33" s="28">
         <v>20</v>
       </c>
-      <c r="I33" s="36">
+      <c r="I33" s="28">
         <v>51</v>
       </c>
-      <c r="J33" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="34">
+      <c r="J33" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="26">
         <v>9</v>
       </c>
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="37" t="s">
+      <c r="C34" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="36"/>
-      <c r="E34" s="35" t="s">
+      <c r="D34" s="28"/>
+      <c r="E34" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F34" s="35"/>
-      <c r="G34" s="36">
+      <c r="F34" s="27"/>
+      <c r="G34" s="28">
         <v>90</v>
       </c>
-      <c r="H34" s="36">
+      <c r="H34" s="28">
         <v>0</v>
       </c>
-      <c r="I34" s="36">
+      <c r="I34" s="28">
         <v>90</v>
       </c>
-      <c r="J34" s="36">
+      <c r="J34" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="43" t="s">
+    <row r="35" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="44">
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="35">
         <f>SUM(D26:D33)</f>
         <v>19</v>
       </c>
-      <c r="E35" s="44">
+      <c r="E35" s="35">
         <f t="shared" ref="E35:J35" si="0">SUM(E26:E33)</f>
         <v>0</v>
       </c>
-      <c r="F35" s="44">
+      <c r="F35" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G35" s="44">
+      <c r="G35" s="35">
         <f>SUM(G26:G33)</f>
         <v>435</v>
       </c>
-      <c r="H35" s="44">
+      <c r="H35" s="35">
         <f t="shared" si="0"/>
         <v>139</v>
       </c>
-      <c r="I35" s="44">
+      <c r="I35" s="35">
         <f t="shared" si="0"/>
         <v>241</v>
       </c>
-      <c r="J35" s="44">
+      <c r="J35" s="35">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:12" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="33" t="s">
+    <row r="36" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="B46" s="33"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="33"/>
-      <c r="I46" s="33"/>
-      <c r="J46" s="33"/>
-    </row>
-    <row r="47" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:12" s="32" customFormat="1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A48" s="34" t="s">
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
+    </row>
+    <row r="47" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:12" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+      <c r="A48" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="34" t="s">
+      <c r="B48" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C48" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="D48" s="34" t="s">
+      <c r="D48" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="E48" s="34" t="s">
+      <c r="E48" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="F48" s="34" t="s">
+      <c r="F48" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="G48" s="34" t="s">
+      <c r="G48" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="H48" s="34" t="s">
+      <c r="H48" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I48" s="34" t="s">
+      <c r="I48" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="J48" s="34" t="s">
+      <c r="J48" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="L48" s="32">
+      <c r="L48" s="25">
         <f>32+15</f>
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="35">
+    <row r="49" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A49" s="27">
         <v>1</v>
       </c>
-      <c r="B49" s="36" t="s">
+      <c r="B49" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="37" t="s">
+      <c r="C49" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D49" s="36">
-        <v>3</v>
-      </c>
-      <c r="E49" s="35" t="s">
+      <c r="D49" s="28">
+        <v>3</v>
+      </c>
+      <c r="E49" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F49" s="35"/>
-      <c r="G49" s="36">
+      <c r="F49" s="27"/>
+      <c r="G49" s="28">
         <v>75</v>
       </c>
-      <c r="H49" s="36">
+      <c r="H49" s="28">
         <v>20</v>
       </c>
-      <c r="I49" s="36">
+      <c r="I49" s="28">
         <v>51</v>
       </c>
-      <c r="J49" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A50" s="35">
+      <c r="J49" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A50" s="27">
         <v>2</v>
       </c>
-      <c r="B50" s="36" t="s">
+      <c r="B50" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C50" s="37" t="s">
+      <c r="C50" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D50" s="36">
-        <v>3</v>
-      </c>
-      <c r="E50" s="35" t="s">
+      <c r="D50" s="28">
+        <v>3</v>
+      </c>
+      <c r="E50" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F50" s="35"/>
-      <c r="G50" s="36">
+      <c r="F50" s="27"/>
+      <c r="G50" s="28">
         <v>75</v>
       </c>
-      <c r="H50" s="36">
+      <c r="H50" s="28">
         <v>20</v>
       </c>
-      <c r="I50" s="36">
+      <c r="I50" s="28">
         <v>51</v>
       </c>
-      <c r="J50" s="36">
-        <v>4</v>
-      </c>
-      <c r="L50" s="32">
+      <c r="J50" s="28">
+        <v>4</v>
+      </c>
+      <c r="L50" s="25">
         <f>91-6</f>
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A51" s="35">
-        <v>3</v>
-      </c>
-      <c r="B51" s="36" t="s">
+    <row r="51" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A51" s="27">
+        <v>3</v>
+      </c>
+      <c r="B51" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="37" t="s">
+      <c r="C51" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D51" s="36">
-        <v>3</v>
-      </c>
-      <c r="E51" s="35" t="s">
+      <c r="D51" s="28">
+        <v>3</v>
+      </c>
+      <c r="E51" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F51" s="35"/>
-      <c r="G51" s="36">
+      <c r="F51" s="27"/>
+      <c r="G51" s="28">
         <v>75</v>
       </c>
-      <c r="H51" s="36">
+      <c r="H51" s="28">
         <v>20</v>
       </c>
-      <c r="I51" s="36">
+      <c r="I51" s="28">
         <v>51</v>
       </c>
-      <c r="J51" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A52" s="35">
-        <v>4</v>
-      </c>
-      <c r="B52" s="36" t="s">
+      <c r="J51" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A52" s="27">
+        <v>4</v>
+      </c>
+      <c r="B52" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C52" s="37" t="s">
+      <c r="C52" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D52" s="36">
-        <v>3</v>
-      </c>
-      <c r="E52" s="35" t="s">
+      <c r="D52" s="28">
+        <v>3</v>
+      </c>
+      <c r="E52" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F52" s="35"/>
-      <c r="G52" s="36">
+      <c r="F52" s="27"/>
+      <c r="G52" s="28">
         <v>75</v>
       </c>
-      <c r="H52" s="36">
+      <c r="H52" s="28">
         <v>20</v>
       </c>
-      <c r="I52" s="36">
+      <c r="I52" s="28">
         <v>51</v>
       </c>
-      <c r="J52" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A53" s="35">
+      <c r="J52" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A53" s="27">
         <v>5</v>
       </c>
-      <c r="B53" s="36" t="s">
+      <c r="B53" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C53" s="37" t="s">
+      <c r="C53" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="D53" s="36">
-        <v>3</v>
-      </c>
-      <c r="E53" s="35" t="s">
+      <c r="D53" s="28">
+        <v>3</v>
+      </c>
+      <c r="E53" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F53" s="35"/>
-      <c r="G53" s="36">
+      <c r="F53" s="27"/>
+      <c r="G53" s="28">
         <v>75</v>
       </c>
-      <c r="H53" s="36">
+      <c r="H53" s="28">
         <v>20</v>
       </c>
-      <c r="I53" s="36">
+      <c r="I53" s="28">
         <v>51</v>
       </c>
-      <c r="J53" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="35">
+      <c r="J53" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A54" s="27">
         <v>6</v>
       </c>
-      <c r="B54" s="36" t="s">
+      <c r="B54" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C54" s="37" t="s">
+      <c r="C54" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D54" s="36"/>
-      <c r="E54" s="35" t="s">
+      <c r="D54" s="28"/>
+      <c r="E54" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F54" s="35"/>
-      <c r="G54" s="36">
+      <c r="F54" s="27"/>
+      <c r="G54" s="28">
         <v>90</v>
       </c>
-      <c r="H54" s="36">
+      <c r="H54" s="28">
         <v>0</v>
       </c>
-      <c r="I54" s="36">
+      <c r="I54" s="28">
         <v>90</v>
       </c>
-      <c r="J54" s="36">
+      <c r="J54" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="43" t="s">
+    <row r="55" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B55" s="43"/>
-      <c r="C55" s="43"/>
-      <c r="D55" s="44">
+      <c r="B55" s="57"/>
+      <c r="C55" s="57"/>
+      <c r="D55" s="35">
         <f>SUM(D49:D53)</f>
         <v>15</v>
       </c>
-      <c r="E55" s="44">
+      <c r="E55" s="35">
         <f t="shared" ref="E55:J55" si="1">SUM(E49:E53)</f>
         <v>0</v>
       </c>
-      <c r="F55" s="44">
+      <c r="F55" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G55" s="44">
+      <c r="G55" s="35">
         <f t="shared" si="1"/>
         <v>375</v>
       </c>
-      <c r="H55" s="44">
+      <c r="H55" s="35">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="I55" s="44">
+      <c r="I55" s="35">
         <f t="shared" si="1"/>
         <v>255</v>
       </c>
-      <c r="J55" s="44">
+      <c r="J55" s="35">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:12" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="33" t="s">
+    <row r="56" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="B57" s="33"/>
-      <c r="C57" s="33"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="33"/>
-      <c r="I57" s="33"/>
-      <c r="J57" s="33"/>
-    </row>
-    <row r="58" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:12" s="32" customFormat="1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A59" s="34" t="s">
+      <c r="B57" s="53"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="53"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="53"/>
+      <c r="H57" s="53"/>
+      <c r="I57" s="53"/>
+      <c r="J57" s="53"/>
+    </row>
+    <row r="58" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:12" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+      <c r="A59" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B59" s="34" t="s">
+      <c r="B59" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="34" t="s">
+      <c r="C59" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="D59" s="34" t="s">
+      <c r="D59" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="E59" s="34" t="s">
+      <c r="E59" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="F59" s="34" t="s">
+      <c r="F59" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="G59" s="34" t="s">
+      <c r="G59" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="H59" s="34" t="s">
+      <c r="H59" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I59" s="34" t="s">
+      <c r="I59" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="J59" s="34" t="s">
+      <c r="J59" s="26" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="60" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A60" s="35">
+    <row r="60" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A60" s="27">
         <v>1</v>
       </c>
-      <c r="B60" s="36" t="s">
+      <c r="B60" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C60" s="37" t="s">
+      <c r="C60" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D60" s="36">
+      <c r="D60" s="28">
         <v>1</v>
       </c>
-      <c r="E60" s="35" t="s">
+      <c r="E60" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F60" s="35"/>
-      <c r="G60" s="36">
+      <c r="F60" s="27"/>
+      <c r="G60" s="28">
         <v>45</v>
       </c>
-      <c r="H60" s="36">
+      <c r="H60" s="28">
         <v>0</v>
       </c>
-      <c r="I60" s="36">
+      <c r="I60" s="28">
         <v>45</v>
       </c>
-      <c r="J60" s="36">
+      <c r="J60" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A61" s="35">
+    <row r="61" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A61" s="27">
         <v>2</v>
       </c>
-      <c r="B61" s="36" t="s">
+      <c r="B61" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C61" s="37" t="s">
+      <c r="C61" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D61" s="36">
-        <v>3</v>
-      </c>
-      <c r="E61" s="35" t="s">
+      <c r="D61" s="28">
+        <v>3</v>
+      </c>
+      <c r="E61" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F61" s="35"/>
-      <c r="G61" s="36">
+      <c r="F61" s="27"/>
+      <c r="G61" s="28">
         <v>75</v>
       </c>
-      <c r="H61" s="36">
+      <c r="H61" s="28">
         <v>20</v>
       </c>
-      <c r="I61" s="36">
+      <c r="I61" s="28">
         <v>51</v>
       </c>
-      <c r="J61" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A62" s="35">
-        <v>3</v>
-      </c>
-      <c r="B62" s="36" t="s">
+      <c r="J61" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A62" s="27">
+        <v>3</v>
+      </c>
+      <c r="B62" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C62" s="37" t="s">
+      <c r="C62" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D62" s="36">
-        <v>3</v>
-      </c>
-      <c r="E62" s="35" t="s">
+      <c r="D62" s="28">
+        <v>3</v>
+      </c>
+      <c r="E62" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F62" s="35"/>
-      <c r="G62" s="36">
+      <c r="F62" s="27"/>
+      <c r="G62" s="28">
         <v>75</v>
       </c>
-      <c r="H62" s="36">
+      <c r="H62" s="28">
         <v>20</v>
       </c>
-      <c r="I62" s="36">
+      <c r="I62" s="28">
         <v>51</v>
       </c>
-      <c r="J62" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="35">
-        <v>4</v>
-      </c>
-      <c r="B63" s="36" t="s">
+      <c r="J62" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A63" s="27">
+        <v>4</v>
+      </c>
+      <c r="B63" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="37" t="s">
+      <c r="C63" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D63" s="36">
-        <v>3</v>
-      </c>
-      <c r="E63" s="35" t="s">
+      <c r="D63" s="28">
+        <v>3</v>
+      </c>
+      <c r="E63" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F63" s="35"/>
-      <c r="G63" s="36">
+      <c r="F63" s="27"/>
+      <c r="G63" s="28">
         <v>75</v>
       </c>
-      <c r="H63" s="36">
+      <c r="H63" s="28">
         <v>20</v>
       </c>
-      <c r="I63" s="36">
+      <c r="I63" s="28">
         <v>51</v>
       </c>
-      <c r="J63" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A64" s="35">
+      <c r="J63" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A64" s="27">
         <v>5</v>
       </c>
-      <c r="B64" s="36" t="s">
+      <c r="B64" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C64" s="37" t="s">
+      <c r="C64" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="36">
-        <v>3</v>
-      </c>
-      <c r="E64" s="35" t="s">
+      <c r="D64" s="28">
+        <v>3</v>
+      </c>
+      <c r="E64" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F64" s="35"/>
-      <c r="G64" s="36">
+      <c r="F64" s="27"/>
+      <c r="G64" s="28">
         <v>75</v>
       </c>
-      <c r="H64" s="36">
+      <c r="H64" s="28">
         <v>20</v>
       </c>
-      <c r="I64" s="36">
+      <c r="I64" s="28">
         <v>51</v>
       </c>
-      <c r="J64" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="35">
+      <c r="J64" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A65" s="27">
         <v>6</v>
       </c>
-      <c r="B65" s="36" t="s">
+      <c r="B65" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C65" s="37" t="s">
+      <c r="C65" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D65" s="36">
-        <v>3</v>
-      </c>
-      <c r="E65" s="35" t="s">
+      <c r="D65" s="28">
+        <v>3</v>
+      </c>
+      <c r="E65" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F65" s="35"/>
-      <c r="G65" s="36">
+      <c r="F65" s="27"/>
+      <c r="G65" s="28">
         <v>75</v>
       </c>
-      <c r="H65" s="36">
+      <c r="H65" s="28">
         <v>20</v>
       </c>
-      <c r="I65" s="36">
+      <c r="I65" s="28">
         <v>51</v>
       </c>
-      <c r="J65" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="35">
+      <c r="J65" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A66" s="27">
         <v>7</v>
       </c>
-      <c r="B66" s="36" t="s">
+      <c r="B66" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C66" s="37" t="s">
+      <c r="C66" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D66" s="36"/>
-      <c r="E66" s="35" t="s">
+      <c r="D66" s="28"/>
+      <c r="E66" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F66" s="35"/>
-      <c r="G66" s="36">
+      <c r="F66" s="27"/>
+      <c r="G66" s="28">
         <v>90</v>
       </c>
-      <c r="H66" s="36">
+      <c r="H66" s="28">
         <v>0</v>
       </c>
-      <c r="I66" s="36">
+      <c r="I66" s="28">
         <v>90</v>
       </c>
-      <c r="J66" s="36">
+      <c r="J66" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="43" t="s">
+    <row r="67" spans="1:10" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="43"/>
-      <c r="C67" s="43"/>
-      <c r="D67" s="46">
+      <c r="B67" s="57"/>
+      <c r="C67" s="57"/>
+      <c r="D67" s="37">
         <f>SUM(D60:D65)</f>
         <v>16</v>
       </c>
-      <c r="E67" s="46">
+      <c r="E67" s="37">
         <f t="shared" ref="E67:J67" si="2">SUM(E60:E65)</f>
         <v>0</v>
       </c>
-      <c r="F67" s="46">
+      <c r="F67" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G67" s="46">
+      <c r="G67" s="37">
         <f t="shared" si="2"/>
         <v>420</v>
       </c>
-      <c r="H67" s="46">
+      <c r="H67" s="37">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="I67" s="46">
+      <c r="I67" s="37">
         <f t="shared" si="2"/>
         <v>300</v>
       </c>
-      <c r="J67" s="46">
+      <c r="J67" s="37">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:10" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="33" t="s">
+    <row r="68" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="1:10" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="B69" s="33"/>
-      <c r="C69" s="33"/>
-      <c r="D69" s="33"/>
-      <c r="E69" s="33"/>
-      <c r="F69" s="33"/>
-      <c r="G69" s="33"/>
-      <c r="H69" s="33"/>
-      <c r="I69" s="33"/>
-      <c r="J69" s="33"/>
-    </row>
-    <row r="70" spans="1:10" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:10" s="32" customFormat="1" ht="63" x14ac:dyDescent="0.2">
-      <c r="A71" s="34" t="s">
+      <c r="B69" s="53"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="53"/>
+      <c r="E69" s="53"/>
+      <c r="F69" s="53"/>
+      <c r="G69" s="53"/>
+      <c r="H69" s="53"/>
+      <c r="I69" s="53"/>
+      <c r="J69" s="53"/>
+    </row>
+    <row r="70" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="1:10" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+      <c r="A71" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B71" s="34" t="s">
+      <c r="B71" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C71" s="34" t="s">
+      <c r="C71" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="D71" s="34" t="s">
+      <c r="D71" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="E71" s="34" t="s">
+      <c r="E71" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="F71" s="34" t="s">
+      <c r="F71" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="G71" s="34" t="s">
+      <c r="G71" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="H71" s="34" t="s">
+      <c r="H71" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="I71" s="34" t="s">
+      <c r="I71" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="J71" s="34" t="s">
+      <c r="J71" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="72" spans="1:10" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A72" s="35">
+    <row r="72" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A72" s="27">
         <v>1</v>
       </c>
-      <c r="B72" s="36" t="s">
+      <c r="B72" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C72" s="37" t="s">
+      <c r="C72" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="D72" s="36">
+      <c r="D72" s="28">
         <v>1</v>
       </c>
-      <c r="F72" s="35" t="s">
+      <c r="F72" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="G72" s="36">
+      <c r="G72" s="28">
         <v>45</v>
       </c>
-      <c r="H72" s="36">
+      <c r="H72" s="28">
         <v>0</v>
       </c>
-      <c r="I72" s="36">
+      <c r="I72" s="28">
         <v>45</v>
       </c>
-      <c r="J72" s="36">
+      <c r="J72" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A73" s="35">
+    <row r="73" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A73" s="27">
         <v>2</v>
       </c>
-      <c r="B73" s="36" t="s">
+      <c r="B73" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C73" s="37" t="s">
+      <c r="C73" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D73" s="36">
-        <v>3</v>
-      </c>
-      <c r="E73" s="35" t="s">
+      <c r="D73" s="28">
+        <v>3</v>
+      </c>
+      <c r="E73" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F73" s="35"/>
-      <c r="G73" s="36">
+      <c r="F73" s="27"/>
+      <c r="G73" s="28">
         <v>75</v>
       </c>
-      <c r="H73" s="36">
+      <c r="H73" s="28">
         <v>20</v>
       </c>
-      <c r="I73" s="36">
+      <c r="I73" s="28">
         <v>51</v>
       </c>
-      <c r="J73" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A74" s="35">
-        <v>3</v>
-      </c>
-      <c r="B74" s="36" t="s">
+      <c r="J73" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A74" s="27">
+        <v>3</v>
+      </c>
+      <c r="B74" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C74" s="37" t="s">
+      <c r="C74" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="D74" s="36">
+      <c r="D74" s="28">
         <v>2</v>
       </c>
-      <c r="E74" s="35" t="s">
+      <c r="E74" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F74" s="35"/>
-      <c r="G74" s="36">
+      <c r="F74" s="27"/>
+      <c r="G74" s="28">
         <v>45</v>
       </c>
-      <c r="H74" s="36">
+      <c r="H74" s="28">
         <v>17</v>
       </c>
-      <c r="I74" s="36">
+      <c r="I74" s="28">
         <v>25</v>
       </c>
-      <c r="J74" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A75" s="35">
-        <v>4</v>
-      </c>
-      <c r="B75" s="36" t="s">
+      <c r="J74" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A75" s="27">
+        <v>4</v>
+      </c>
+      <c r="B75" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C75" s="37" t="s">
+      <c r="C75" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="D75" s="36">
+      <c r="D75" s="28">
         <v>2</v>
       </c>
-      <c r="E75" s="35" t="s">
+      <c r="E75" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="F75" s="35"/>
-      <c r="G75" s="36">
+      <c r="F75" s="27"/>
+      <c r="G75" s="28">
         <v>45</v>
       </c>
-      <c r="H75" s="36">
+      <c r="H75" s="28">
         <v>17</v>
       </c>
-      <c r="I75" s="36">
+      <c r="I75" s="28">
         <v>25</v>
       </c>
-      <c r="J75" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A76" s="35">
+      <c r="J75" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A76" s="27">
         <v>5</v>
       </c>
-      <c r="B76" s="47" t="s">
+      <c r="B76" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="C76" s="48" t="s">
+      <c r="C76" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="D76" s="49">
+      <c r="D76" s="40">
         <v>6</v>
       </c>
-      <c r="E76" s="50" t="s">
+      <c r="E76" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="F76" s="50"/>
-      <c r="G76" s="49">
+      <c r="F76" s="41"/>
+      <c r="G76" s="40">
         <f>6*45</f>
         <v>270</v>
       </c>
-      <c r="H76" s="49">
+      <c r="H76" s="40">
         <v>0</v>
       </c>
-      <c r="I76" s="49">
+      <c r="I76" s="40">
         <f>6*45</f>
         <v>270</v>
       </c>
-      <c r="J76" s="49">
+      <c r="J76" s="40">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="32" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="51">
+    <row r="77" spans="1:10" s="25" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="59">
         <v>6</v>
       </c>
-      <c r="B77" s="36" t="s">
+      <c r="B77" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C77" s="37" t="s">
+      <c r="C77" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D77" s="36">
+      <c r="D77" s="28">
         <v>2</v>
       </c>
-      <c r="E77" s="35"/>
-      <c r="F77" s="35" t="s">
+      <c r="E77" s="27"/>
+      <c r="F77" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="G77" s="36">
+      <c r="G77" s="28">
         <v>45</v>
       </c>
-      <c r="H77" s="36">
+      <c r="H77" s="28">
         <v>17</v>
       </c>
-      <c r="I77" s="36">
+      <c r="I77" s="28">
         <v>25</v>
       </c>
-      <c r="J77" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" s="32" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="52"/>
-      <c r="B78" s="36" t="s">
+      <c r="J77" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" s="25" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="60"/>
+      <c r="B78" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C78" s="37" t="s">
+      <c r="C78" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D78" s="36">
+      <c r="D78" s="28">
         <v>2</v>
       </c>
-      <c r="E78" s="35"/>
-      <c r="F78" s="35" t="s">
+      <c r="E78" s="27"/>
+      <c r="F78" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="G78" s="36">
+      <c r="G78" s="28">
         <v>45</v>
       </c>
-      <c r="H78" s="36">
+      <c r="H78" s="28">
         <v>17</v>
       </c>
-      <c r="I78" s="36">
+      <c r="I78" s="28">
         <v>25</v>
       </c>
-      <c r="J78" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" s="32" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="52"/>
-      <c r="B79" s="36" t="s">
+      <c r="J78" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" s="25" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="60"/>
+      <c r="B79" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C79" s="37" t="s">
+      <c r="C79" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="D79" s="36">
+      <c r="D79" s="28">
         <v>2</v>
       </c>
-      <c r="E79" s="35"/>
-      <c r="F79" s="35" t="s">
+      <c r="E79" s="27"/>
+      <c r="F79" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="G79" s="36">
+      <c r="G79" s="28">
         <v>45</v>
       </c>
-      <c r="H79" s="36">
+      <c r="H79" s="28">
         <v>17</v>
       </c>
-      <c r="I79" s="36">
+      <c r="I79" s="28">
         <v>25</v>
       </c>
-      <c r="J79" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" s="32" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="52"/>
-      <c r="B80" s="36" t="s">
+      <c r="J79" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="25" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="60"/>
+      <c r="B80" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C80" s="37" t="s">
+      <c r="C80" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D80" s="36">
+      <c r="D80" s="28">
         <v>2</v>
       </c>
-      <c r="E80" s="35"/>
-      <c r="F80" s="35" t="s">
+      <c r="E80" s="27"/>
+      <c r="F80" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="G80" s="36">
+      <c r="G80" s="28">
         <v>45</v>
       </c>
-      <c r="H80" s="36">
+      <c r="H80" s="28">
         <v>17</v>
       </c>
-      <c r="I80" s="36">
+      <c r="I80" s="28">
         <v>25</v>
       </c>
-      <c r="J80" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="52"/>
-      <c r="B81" s="36" t="s">
+      <c r="J80" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A81" s="60"/>
+      <c r="B81" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C81" s="37" t="s">
+      <c r="C81" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D81" s="36">
+      <c r="D81" s="28">
         <v>2</v>
       </c>
-      <c r="E81" s="35"/>
-      <c r="F81" s="35" t="s">
+      <c r="E81" s="27"/>
+      <c r="F81" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="G81" s="36">
+      <c r="G81" s="28">
         <v>45</v>
       </c>
-      <c r="H81" s="36">
+      <c r="H81" s="28">
         <v>17</v>
       </c>
-      <c r="I81" s="36">
+      <c r="I81" s="28">
         <v>25</v>
       </c>
-      <c r="J81" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" s="32" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A82" s="52"/>
-      <c r="B82" s="36" t="s">
+      <c r="J81" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A82" s="60"/>
+      <c r="B82" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C82" s="37" t="s">
+      <c r="C82" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="D82" s="36">
+      <c r="D82" s="28">
         <v>2</v>
       </c>
-      <c r="E82" s="35"/>
-      <c r="F82" s="35" t="s">
+      <c r="E82" s="27"/>
+      <c r="F82" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="G82" s="36">
+      <c r="G82" s="28">
         <v>45</v>
       </c>
-      <c r="H82" s="36">
+      <c r="H82" s="28">
         <v>17</v>
       </c>
-      <c r="I82" s="36">
+      <c r="I82" s="28">
         <v>25</v>
       </c>
-      <c r="J82" s="36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="43" t="s">
+      <c r="J82" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B83" s="43"/>
-      <c r="C83" s="43"/>
-      <c r="D83" s="53">
+      <c r="B83" s="57"/>
+      <c r="C83" s="57"/>
+      <c r="D83" s="42">
         <f>SUM(D72:D77)</f>
         <v>16</v>
       </c>
-      <c r="E83" s="44"/>
-      <c r="F83" s="44"/>
-      <c r="G83" s="46">
+      <c r="E83" s="35"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="37">
         <f>SUM(G72:G77)</f>
         <v>525</v>
       </c>
-      <c r="H83" s="46">
+      <c r="H83" s="37">
         <f t="shared" ref="H83:J83" si="3">SUM(H72:H77)</f>
         <v>71</v>
       </c>
-      <c r="I83" s="46">
+      <c r="I83" s="37">
         <f t="shared" si="3"/>
         <v>441</v>
       </c>
-      <c r="J83" s="46">
+      <c r="J83" s="37">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="D84" s="54" t="s">
+      <c r="D84" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="E84" s="54"/>
-      <c r="F84" s="54"/>
-      <c r="G84" s="54"/>
-      <c r="H84" s="54"/>
-      <c r="I84" s="54"/>
-      <c r="J84" s="54"/>
+      <c r="E84" s="58"/>
+      <c r="F84" s="58"/>
+      <c r="G84" s="58"/>
+      <c r="H84" s="58"/>
+      <c r="I84" s="58"/>
+      <c r="J84" s="58"/>
     </row>
     <row r="85" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A85" s="55" t="s">
+      <c r="A85" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="B85" s="56"/>
-      <c r="C85" s="55"/>
-      <c r="D85" s="57" t="s">
+      <c r="B85" s="44"/>
+      <c r="C85" s="43"/>
+      <c r="D85" s="45" t="s">
         <v>112</v>
       </c>
       <c r="E85" s="17"/>
       <c r="F85" s="17"/>
-      <c r="H85" s="58"/>
-      <c r="I85" s="59" t="s">
+      <c r="H85" s="46"/>
+      <c r="I85" s="47" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A86" s="55"/>
-      <c r="B86" s="56"/>
-      <c r="C86" s="55"/>
-      <c r="D86" s="57"/>
+      <c r="A86" s="43"/>
+      <c r="B86" s="44"/>
+      <c r="C86" s="43"/>
+      <c r="D86" s="45"/>
       <c r="E86" s="17"/>
       <c r="F86" s="17"/>
-      <c r="H86" s="58"/>
-      <c r="I86" s="59"/>
+      <c r="H86" s="46"/>
+      <c r="I86" s="47"/>
     </row>
     <row r="87" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A87" s="55"/>
-      <c r="B87" s="56"/>
-      <c r="C87" s="55"/>
-      <c r="D87" s="57"/>
+      <c r="A87" s="43"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="43"/>
+      <c r="D87" s="45"/>
       <c r="E87" s="17"/>
       <c r="F87" s="17"/>
-      <c r="H87" s="58"/>
-      <c r="I87" s="59"/>
+      <c r="H87" s="46"/>
+      <c r="I87" s="47"/>
     </row>
     <row r="88" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A88" s="60" t="s">
+      <c r="A88" s="48" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D84:J84"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A69:J69"/>
+    <mergeCell ref="A83:C83"/>
+    <mergeCell ref="A77:A82"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="A57:J57"/>
     <mergeCell ref="E2:J2"/>
@@ -6112,11 +6117,6 @@
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A46:J46"/>
     <mergeCell ref="A55:C55"/>
-    <mergeCell ref="D84:J84"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A69:J69"/>
-    <mergeCell ref="A83:C83"/>
-    <mergeCell ref="A77:A82"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="90" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chuc nang bat buoc tu chon
</commit_message>
<xml_diff>
--- a/upload/best_data.xlsx
+++ b/upload/best_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\best_xuly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20280" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="KE HOẠCH GD TIN UD K42" sheetId="2" r:id="rId1"/>
@@ -503,10 +503,10 @@
     </r>
   </si>
   <si>
+    <t>Nghành đào tạo: Tin học ứng dụng    Mã Nghành: 6480205</t>
+  </si>
+  <si>
     <t>Khóa học 42 (2017-2020)</t>
-  </si>
-  <si>
-    <t>Nghành đào tạo: Tin học ứng dụng    Mã Nghành: 1</t>
   </si>
 </sst>
 </file>
@@ -868,23 +868,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -894,6 +882,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1294,7 +1294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:J5"/>
     </sheetView>
   </sheetViews>
@@ -1697,15 +1697,15 @@
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
     </row>
     <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -1713,56 +1713,56 @@
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
     </row>
     <row r="4" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
     </row>
     <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+    </row>
+    <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-    </row>
-    <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
-        <v>141</v>
-      </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
     </row>
     <row r="7" spans="1:16" s="25" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
@@ -1777,18 +1777,18 @@
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:16" s="25" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
     </row>
     <row r="9" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:16" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
@@ -2118,11 +2118,11 @@
       </c>
     </row>
     <row r="20" spans="1:16" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
       <c r="D20" s="35">
         <f>SUM(D11:D19)</f>
         <v>23</v>
@@ -2151,18 +2151,18 @@
     <row r="21" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:16" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="53" t="s">
         <v>137</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
     </row>
     <row r="24" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:16" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
@@ -2463,11 +2463,11 @@
       </c>
     </row>
     <row r="35" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
       <c r="D35" s="35">
         <f>SUM(D26:D33)</f>
         <v>19</v>
@@ -2508,18 +2508,18 @@
     <row r="44" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="54" t="s">
+      <c r="A46" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="B46" s="54"/>
-      <c r="C46" s="54"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="54"/>
-      <c r="F46" s="54"/>
-      <c r="G46" s="54"/>
-      <c r="H46" s="54"/>
-      <c r="I46" s="54"/>
-      <c r="J46" s="54"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
     </row>
     <row r="47" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="48" spans="1:12" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
@@ -2741,11 +2741,11 @@
       </c>
     </row>
     <row r="55" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="53" t="s">
+      <c r="A55" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B55" s="53"/>
-      <c r="C55" s="53"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="57"/>
       <c r="D55" s="35">
         <f>SUM(D49:D53)</f>
         <v>15</v>
@@ -2777,18 +2777,18 @@
     </row>
     <row r="56" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="54" t="s">
+      <c r="A57" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="B57" s="54"/>
-      <c r="C57" s="54"/>
-      <c r="D57" s="54"/>
-      <c r="E57" s="54"/>
-      <c r="F57" s="54"/>
-      <c r="G57" s="54"/>
-      <c r="H57" s="54"/>
-      <c r="I57" s="54"/>
-      <c r="J57" s="54"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="53"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="53"/>
+      <c r="H57" s="53"/>
+      <c r="I57" s="53"/>
+      <c r="J57" s="53"/>
     </row>
     <row r="58" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:12" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
@@ -3032,11 +3032,11 @@
       </c>
     </row>
     <row r="67" spans="1:10" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="53" t="s">
+      <c r="A67" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="53"/>
-      <c r="C67" s="53"/>
+      <c r="B67" s="57"/>
+      <c r="C67" s="57"/>
       <c r="D67" s="37">
         <f>SUM(D60:D65)</f>
         <v>16</v>
@@ -3068,18 +3068,18 @@
     </row>
     <row r="68" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="69" spans="1:10" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="54" t="s">
+      <c r="A69" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="B69" s="54"/>
-      <c r="C69" s="54"/>
-      <c r="D69" s="54"/>
-      <c r="E69" s="54"/>
-      <c r="F69" s="54"/>
-      <c r="G69" s="54"/>
-      <c r="H69" s="54"/>
-      <c r="I69" s="54"/>
-      <c r="J69" s="54"/>
+      <c r="B69" s="53"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="53"/>
+      <c r="E69" s="53"/>
+      <c r="F69" s="53"/>
+      <c r="G69" s="53"/>
+      <c r="H69" s="53"/>
+      <c r="I69" s="53"/>
+      <c r="J69" s="53"/>
     </row>
     <row r="70" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="71" spans="1:10" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
@@ -3266,7 +3266,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" s="25" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="55">
+      <c r="A77" s="59">
         <v>6</v>
       </c>
       <c r="B77" s="28" t="s">
@@ -3296,7 +3296,7 @@
       </c>
     </row>
     <row r="78" spans="1:10" s="25" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="56"/>
+      <c r="A78" s="60"/>
       <c r="B78" s="28" t="s">
         <v>60</v>
       </c>
@@ -3324,7 +3324,7 @@
       </c>
     </row>
     <row r="79" spans="1:10" s="25" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="56"/>
+      <c r="A79" s="60"/>
       <c r="B79" s="28" t="s">
         <v>62</v>
       </c>
@@ -3352,7 +3352,7 @@
       </c>
     </row>
     <row r="80" spans="1:10" s="25" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="56"/>
+      <c r="A80" s="60"/>
       <c r="B80" s="28" t="s">
         <v>64</v>
       </c>
@@ -3380,7 +3380,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="56"/>
+      <c r="A81" s="60"/>
       <c r="B81" s="28" t="s">
         <v>66</v>
       </c>
@@ -3408,7 +3408,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A82" s="56"/>
+      <c r="A82" s="60"/>
       <c r="B82" s="28" t="s">
         <v>68</v>
       </c>
@@ -3436,11 +3436,11 @@
       </c>
     </row>
     <row r="83" spans="1:10" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="53" t="s">
+      <c r="A83" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B83" s="53"/>
-      <c r="C83" s="53"/>
+      <c r="B83" s="57"/>
+      <c r="C83" s="57"/>
       <c r="D83" s="42">
         <f>SUM(D72:D77)</f>
         <v>16</v>
@@ -3465,15 +3465,15 @@
       </c>
     </row>
     <row r="84" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="D84" s="52" t="s">
+      <c r="D84" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="E84" s="52"/>
-      <c r="F84" s="52"/>
-      <c r="G84" s="52"/>
-      <c r="H84" s="52"/>
-      <c r="I84" s="52"/>
-      <c r="J84" s="52"/>
+      <c r="E84" s="58"/>
+      <c r="F84" s="58"/>
+      <c r="G84" s="58"/>
+      <c r="H84" s="58"/>
+      <c r="I84" s="58"/>
+      <c r="J84" s="58"/>
     </row>
     <row r="85" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="43" t="s">
@@ -3518,6 +3518,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D84:J84"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A69:J69"/>
+    <mergeCell ref="A83:C83"/>
+    <mergeCell ref="A77:A82"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="A57:J57"/>
     <mergeCell ref="E2:J2"/>
@@ -3530,11 +3535,6 @@
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A46:J46"/>
     <mergeCell ref="A55:C55"/>
-    <mergeCell ref="D84:J84"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A69:J69"/>
-    <mergeCell ref="A83:C83"/>
-    <mergeCell ref="A77:A82"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="90" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chuc nang KHGD cho truong bo mon
</commit_message>
<xml_diff>
--- a/upload/best_data.xlsx
+++ b/upload/best_data.xlsx
@@ -503,10 +503,10 @@
     </r>
   </si>
   <si>
-    <t>Nghành đào tạo: Tin học ứng dụng    Mã Nghành: 6480205</t>
-  </si>
-  <si>
     <t>Khóa học 42 (2017-2020)</t>
+  </si>
+  <si>
+    <t>Ngành đào tạo: Tin học ứng dụng    Mã Ngành: 6480205</t>
   </si>
 </sst>
 </file>
@@ -859,20 +859,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -883,17 +886,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1294,7 +1294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:J5"/>
     </sheetView>
   </sheetViews>
@@ -1697,15 +1697,15 @@
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
     </row>
     <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -1713,56 +1713,56 @@
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
     </row>
     <row r="4" spans="1:16" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="1:16" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+    </row>
+    <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-    </row>
-    <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
-        <v>142</v>
-      </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
     </row>
     <row r="7" spans="1:16" s="25" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
@@ -1777,18 +1777,18 @@
       <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:16" s="25" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
     </row>
     <row r="9" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:16" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
@@ -2118,11 +2118,11 @@
       </c>
     </row>
     <row r="20" spans="1:16" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="35">
         <f>SUM(D11:D19)</f>
         <v>23</v>
@@ -2151,18 +2151,18 @@
     <row r="21" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:16" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="53"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
     </row>
     <row r="24" spans="1:16" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:16" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
@@ -2463,11 +2463,11 @@
       </c>
     </row>
     <row r="35" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
       <c r="D35" s="35">
         <f>SUM(D26:D33)</f>
         <v>19</v>
@@ -2508,18 +2508,18 @@
     <row r="44" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="53" t="s">
+      <c r="A46" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="B46" s="53"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="51"/>
     </row>
     <row r="47" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="48" spans="1:12" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
@@ -2741,11 +2741,11 @@
       </c>
     </row>
     <row r="55" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="57" t="s">
+      <c r="A55" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B55" s="57"/>
-      <c r="C55" s="57"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="50"/>
       <c r="D55" s="35">
         <f>SUM(D49:D53)</f>
         <v>15</v>
@@ -2777,18 +2777,18 @@
     </row>
     <row r="56" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:12" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="53" t="s">
+      <c r="A57" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="B57" s="53"/>
-      <c r="C57" s="53"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="53"/>
-      <c r="F57" s="53"/>
-      <c r="G57" s="53"/>
-      <c r="H57" s="53"/>
-      <c r="I57" s="53"/>
-      <c r="J57" s="53"/>
+      <c r="B57" s="51"/>
+      <c r="C57" s="51"/>
+      <c r="D57" s="51"/>
+      <c r="E57" s="51"/>
+      <c r="F57" s="51"/>
+      <c r="G57" s="51"/>
+      <c r="H57" s="51"/>
+      <c r="I57" s="51"/>
+      <c r="J57" s="51"/>
     </row>
     <row r="58" spans="1:12" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:12" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
@@ -3032,11 +3032,11 @@
       </c>
     </row>
     <row r="67" spans="1:10" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="57" t="s">
+      <c r="A67" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="57"/>
-      <c r="C67" s="57"/>
+      <c r="B67" s="50"/>
+      <c r="C67" s="50"/>
       <c r="D67" s="37">
         <f>SUM(D60:D65)</f>
         <v>16</v>
@@ -3068,18 +3068,18 @@
     </row>
     <row r="68" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="69" spans="1:10" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="53" t="s">
+      <c r="A69" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="B69" s="53"/>
-      <c r="C69" s="53"/>
-      <c r="D69" s="53"/>
-      <c r="E69" s="53"/>
-      <c r="F69" s="53"/>
-      <c r="G69" s="53"/>
-      <c r="H69" s="53"/>
-      <c r="I69" s="53"/>
-      <c r="J69" s="53"/>
+      <c r="B69" s="51"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="51"/>
+      <c r="E69" s="51"/>
+      <c r="F69" s="51"/>
+      <c r="G69" s="51"/>
+      <c r="H69" s="51"/>
+      <c r="I69" s="51"/>
+      <c r="J69" s="51"/>
     </row>
     <row r="70" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2"/>
     <row r="71" spans="1:10" s="25" customFormat="1" ht="63" x14ac:dyDescent="0.2">
@@ -3266,7 +3266,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" s="25" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="59">
+      <c r="A77" s="52">
         <v>6</v>
       </c>
       <c r="B77" s="28" t="s">
@@ -3296,7 +3296,7 @@
       </c>
     </row>
     <row r="78" spans="1:10" s="25" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="60"/>
+      <c r="A78" s="53"/>
       <c r="B78" s="28" t="s">
         <v>60</v>
       </c>
@@ -3324,7 +3324,7 @@
       </c>
     </row>
     <row r="79" spans="1:10" s="25" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="60"/>
+      <c r="A79" s="53"/>
       <c r="B79" s="28" t="s">
         <v>62</v>
       </c>
@@ -3352,7 +3352,7 @@
       </c>
     </row>
     <row r="80" spans="1:10" s="25" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="60"/>
+      <c r="A80" s="53"/>
       <c r="B80" s="28" t="s">
         <v>64</v>
       </c>
@@ -3380,7 +3380,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="60"/>
+      <c r="A81" s="53"/>
       <c r="B81" s="28" t="s">
         <v>66</v>
       </c>
@@ -3408,7 +3408,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" s="25" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A82" s="60"/>
+      <c r="A82" s="53"/>
       <c r="B82" s="28" t="s">
         <v>68</v>
       </c>
@@ -3436,11 +3436,11 @@
       </c>
     </row>
     <row r="83" spans="1:10" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="57" t="s">
+      <c r="A83" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B83" s="57"/>
-      <c r="C83" s="57"/>
+      <c r="B83" s="50"/>
+      <c r="C83" s="50"/>
       <c r="D83" s="42">
         <f>SUM(D72:D77)</f>
         <v>16</v>
@@ -3465,15 +3465,15 @@
       </c>
     </row>
     <row r="84" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="D84" s="58" t="s">
+      <c r="D84" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="E84" s="58"/>
-      <c r="F84" s="58"/>
-      <c r="G84" s="58"/>
-      <c r="H84" s="58"/>
-      <c r="I84" s="58"/>
-      <c r="J84" s="58"/>
+      <c r="E84" s="49"/>
+      <c r="F84" s="49"/>
+      <c r="G84" s="49"/>
+      <c r="H84" s="49"/>
+      <c r="I84" s="49"/>
+      <c r="J84" s="49"/>
     </row>
     <row r="85" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="43" t="s">
@@ -3518,11 +3518,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D84:J84"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A69:J69"/>
-    <mergeCell ref="A83:C83"/>
-    <mergeCell ref="A77:A82"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="A57:J57"/>
     <mergeCell ref="E2:J2"/>
@@ -3535,6 +3530,11 @@
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A46:J46"/>
     <mergeCell ref="A55:C55"/>
+    <mergeCell ref="D84:J84"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A69:J69"/>
+    <mergeCell ref="A83:C83"/>
+    <mergeCell ref="A77:A82"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="90" orientation="portrait" r:id="rId1"/>
@@ -3559,29 +3559,29 @@
   <sheetData>
     <row r="1" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
     </row>
     <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="51"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="49"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="3" t="s">
         <v>90</v>
       </c>
@@ -4829,10 +4829,10 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="50"/>
+      <c r="C48" s="59"/>
       <c r="D48" s="3">
         <f>SUM(D4+D11)</f>
         <v>83</v>
@@ -4891,29 +4891,29 @@
   <sheetData>
     <row r="1" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
     </row>
     <row r="3" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="51"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="49"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="3" t="s">
         <v>90</v>
       </c>
@@ -6080,10 +6080,10 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="50"/>
+      <c r="C48" s="59"/>
       <c r="D48" s="3">
         <f>SUM(D4+D11)</f>
         <v>83</v>

</xml_diff>